<commit_message>
Crear la lista de genes
</commit_message>
<xml_diff>
--- a/CHGenesOrdenadosConVecinos.xlsx
+++ b/CHGenesOrdenadosConVecinos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ana\Desktop\PC2_LP2_UNALM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\51920\Desktop\PC2-LP\PC2_LP2_UNALM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F9FD56-D0EA-4334-8016-9726E85FACE3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1E95EF-D537-430F-86B4-CD6D7AF7F1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1116,8 +1116,8 @@
   </sheetPr>
   <dimension ref="A1:V214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1145,47 +1145,43 @@
       <c r="G1" s="31"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:22" ht="14.4">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="5">
-        <v>32091689</v>
-      </c>
-      <c r="E2" s="5">
-        <v>32091761</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
+    <row r="2" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:22" ht="14.4">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="12"/>
       <c r="D3" s="5">
-        <v>32837131</v>
+        <v>32091689</v>
       </c>
       <c r="E3" s="5">
-        <v>32838076</v>
+        <v>32091761</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1207,15 +1203,15 @@
     </row>
     <row r="4" spans="1:22" ht="14.4">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="12"/>
       <c r="D4" s="5">
-        <v>33089112</v>
+        <v>32837131</v>
       </c>
       <c r="E4" s="5">
-        <v>33090132</v>
+        <v>32838076</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1237,15 +1233,15 @@
     </row>
     <row r="5" spans="1:22" ht="14.4">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="12"/>
       <c r="D5" s="5">
-        <v>33764252</v>
+        <v>33089112</v>
       </c>
       <c r="E5" s="5">
-        <v>33768221</v>
+        <v>33090132</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -1267,15 +1263,15 @@
     </row>
     <row r="6" spans="1:22" ht="14.4">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="12"/>
       <c r="D6" s="5">
-        <v>33810174</v>
+        <v>33764252</v>
       </c>
       <c r="E6" s="5">
-        <v>33811741</v>
+        <v>33768221</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -1297,19 +1293,19 @@
     </row>
     <row r="7" spans="1:22" ht="14.4">
       <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="13"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="5">
-        <v>33882149</v>
+        <v>33810174</v>
       </c>
       <c r="E7" s="5">
-        <v>33934641</v>
-      </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+        <v>33811741</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1327,15 +1323,15 @@
     </row>
     <row r="8" spans="1:22" ht="14.4">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="13"/>
       <c r="D8" s="5">
-        <v>34199383</v>
+        <v>33882149</v>
       </c>
       <c r="E8" s="5">
-        <v>34231630</v>
+        <v>33934641</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -1355,17 +1351,17 @@
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A9" s="27" t="s">
-        <v>17</v>
+    <row r="9" spans="1:22" ht="14.4">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="13"/>
       <c r="D9" s="5">
-        <v>34235896</v>
+        <v>34199383</v>
       </c>
       <c r="E9" s="5">
-        <v>34251973</v>
+        <v>34231630</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
@@ -1385,17 +1381,17 @@
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
     </row>
-    <row r="10" spans="1:22" ht="14.4">
+    <row r="10" spans="1:22" ht="15.75" customHeight="1">
       <c r="A10" s="27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="13"/>
       <c r="D10" s="5">
-        <v>34811253</v>
+        <v>34235896</v>
       </c>
       <c r="E10" s="5">
-        <v>34812505</v>
+        <v>34251973</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
@@ -1417,15 +1413,15 @@
     </row>
     <row r="11" spans="1:22" ht="14.4">
       <c r="A11" s="27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="5">
-        <v>34826096</v>
+        <v>34811253</v>
       </c>
       <c r="E11" s="5">
-        <v>34855603</v>
+        <v>34812505</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -1447,15 +1443,15 @@
     </row>
     <row r="12" spans="1:22" ht="14.4">
       <c r="A12" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="14"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="5">
-        <v>34857740</v>
+        <v>34826096</v>
       </c>
       <c r="E12" s="5">
-        <v>34864667</v>
+        <v>34855603</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
@@ -1477,15 +1473,15 @@
     </row>
     <row r="13" spans="1:22" ht="14.4">
       <c r="A13" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="13"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="5">
-        <v>34864860</v>
+        <v>34857740</v>
       </c>
       <c r="E13" s="5">
-        <v>34953982</v>
+        <v>34864667</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
@@ -1507,19 +1503,19 @@
     </row>
     <row r="14" spans="1:22" ht="14.4">
       <c r="A14" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="14"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="5">
-        <v>34960381</v>
+        <v>34864860</v>
       </c>
       <c r="E14" s="5">
-        <v>34968544</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+        <v>34953982</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1537,15 +1533,15 @@
     </row>
     <row r="15" spans="1:22" ht="14.4">
       <c r="A15" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="11"/>
-      <c r="C15" s="13"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="5">
-        <v>34994565</v>
+        <v>34960381</v>
       </c>
       <c r="E15" s="5">
-        <v>34996018</v>
+        <v>34968544</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1567,19 +1563,19 @@
     </row>
     <row r="16" spans="1:22" ht="14.4">
       <c r="A16" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="11"/>
-      <c r="C16" s="14"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="5">
-        <v>69289222</v>
+        <v>34994565</v>
       </c>
       <c r="E16" s="5">
-        <v>69431839</v>
-      </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
+        <v>34996018</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1597,19 +1593,19 @@
     </row>
     <row r="17" spans="1:22" ht="14.4">
       <c r="A17" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="12"/>
+        <v>24</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="5">
-        <v>69413344</v>
+        <v>69289222</v>
       </c>
       <c r="E17" s="5">
-        <v>69418230</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+        <v>69431839</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1627,19 +1623,19 @@
     </row>
     <row r="18" spans="1:22" ht="14.4">
       <c r="A18" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="5">
-        <v>69442967</v>
+        <v>69413344</v>
       </c>
       <c r="E18" s="5">
-        <v>69586809</v>
-      </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
+        <v>69418230</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -1657,15 +1653,15 @@
     </row>
     <row r="19" spans="1:22" ht="14.4">
       <c r="A19" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="11"/>
-      <c r="C19" s="14"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="5">
-        <v>69656519</v>
+        <v>69442967</v>
       </c>
       <c r="E19" s="5">
-        <v>69708647</v>
+        <v>69586809</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
@@ -1687,15 +1683,15 @@
     </row>
     <row r="20" spans="1:22" ht="14.4">
       <c r="A20" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="14"/>
       <c r="D20" s="5">
-        <v>69727101</v>
+        <v>69656519</v>
       </c>
       <c r="E20" s="5">
-        <v>69826032</v>
+        <v>69708647</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
@@ -1717,15 +1713,15 @@
     </row>
     <row r="21" spans="1:22" ht="14.4">
       <c r="A21" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="14"/>
       <c r="D21" s="5">
-        <v>69881877</v>
+        <v>69727101</v>
       </c>
       <c r="E21" s="5">
-        <v>69933388</v>
+        <v>69826032</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
@@ -1747,15 +1743,15 @@
     </row>
     <row r="22" spans="1:22" ht="14.4">
       <c r="A22" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="16"/>
+        <v>29</v>
+      </c>
+      <c r="B22" s="11"/>
       <c r="C22" s="14"/>
       <c r="D22" s="5">
-        <v>69937555</v>
+        <v>69881877</v>
       </c>
       <c r="E22" s="5">
-        <v>69941662</v>
+        <v>69933388</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -1777,15 +1773,15 @@
     </row>
     <row r="23" spans="1:22" ht="14.4">
       <c r="A23" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="14"/>
       <c r="D23" s="5">
-        <v>69941767</v>
+        <v>69937555</v>
       </c>
       <c r="E23" s="5">
-        <v>69990604</v>
+        <v>69941662</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -1807,15 +1803,15 @@
     </row>
     <row r="24" spans="1:22" ht="14.4">
       <c r="A24" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="14"/>
       <c r="D24" s="5">
-        <v>69990461</v>
+        <v>69941767</v>
       </c>
       <c r="E24" s="5">
-        <v>70101362</v>
+        <v>69990604</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -1837,15 +1833,15 @@
     </row>
     <row r="25" spans="1:22" ht="14.4">
       <c r="A25" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="16"/>
-      <c r="C25" s="15"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="5">
-        <v>70107479</v>
+        <v>69990461</v>
       </c>
       <c r="E25" s="5">
-        <v>70139011</v>
+        <v>70101362</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
@@ -1867,15 +1863,15 @@
     </row>
     <row r="26" spans="1:22" ht="14.4">
       <c r="A26" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="16"/>
-      <c r="C26" s="14"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="5">
-        <v>70150265</v>
+        <v>70107479</v>
       </c>
       <c r="E26" s="5">
-        <v>70202391</v>
+        <v>70139011</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
@@ -1897,15 +1893,15 @@
     </row>
     <row r="27" spans="1:22" ht="14.4">
       <c r="A27" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="16"/>
-      <c r="C27" s="13"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="5">
-        <v>70225887</v>
+        <v>70150265</v>
       </c>
       <c r="E27" s="5">
-        <v>70241268</v>
+        <v>70202391</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
@@ -1927,15 +1923,15 @@
     </row>
     <row r="28" spans="1:22" ht="14.4">
       <c r="A28" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="13"/>
       <c r="D28" s="5">
-        <v>70248605</v>
+        <v>70225887</v>
       </c>
       <c r="E28" s="5">
-        <v>70298576</v>
+        <v>70241268</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
@@ -1957,15 +1953,15 @@
     </row>
     <row r="29" spans="1:22" ht="14.4">
       <c r="A29" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="16"/>
-      <c r="C29" s="15"/>
+      <c r="C29" s="13"/>
       <c r="D29" s="5">
-        <v>70353419</v>
+        <v>70248605</v>
       </c>
       <c r="E29" s="5">
-        <v>70394458</v>
+        <v>70298576</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -1987,15 +1983,15 @@
     </row>
     <row r="30" spans="1:22" ht="14.4">
       <c r="A30" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="16"/>
-      <c r="C30" s="14"/>
+      <c r="C30" s="15"/>
       <c r="D30" s="5">
-        <v>70405851</v>
+        <v>70353419</v>
       </c>
       <c r="E30" s="5">
-        <v>70553035</v>
+        <v>70394458</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
@@ -2017,15 +2013,15 @@
     </row>
     <row r="31" spans="1:22" ht="14.4">
       <c r="A31" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="16"/>
       <c r="C31" s="14"/>
       <c r="D31" s="5">
-        <v>70543190</v>
+        <v>70405851</v>
       </c>
       <c r="E31" s="5">
-        <v>70555784</v>
+        <v>70553035</v>
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -2047,15 +2043,15 @@
     </row>
     <row r="32" spans="1:22" ht="14.4">
       <c r="A32" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="16"/>
       <c r="C32" s="14"/>
       <c r="D32" s="5">
-        <v>70563308</v>
+        <v>70543190</v>
       </c>
       <c r="E32" s="5">
-        <v>70580733</v>
+        <v>70555784</v>
       </c>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
@@ -2077,15 +2073,15 @@
     </row>
     <row r="33" spans="1:22" ht="14.4">
       <c r="A33" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="16"/>
       <c r="C33" s="14"/>
       <c r="D33" s="5">
-        <v>70580065</v>
+        <v>70563308</v>
       </c>
       <c r="E33" s="5">
-        <v>70627900</v>
+        <v>70580733</v>
       </c>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -2107,19 +2103,19 @@
     </row>
     <row r="34" spans="1:22" ht="14.4">
       <c r="A34" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="13"/>
+        <v>41</v>
+      </c>
+      <c r="B34" s="16"/>
+      <c r="C34" s="14"/>
       <c r="D34" s="5">
-        <v>70629609</v>
+        <v>70580065</v>
       </c>
       <c r="E34" s="5">
-        <v>70655281</v>
-      </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
+        <v>70627900</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -2137,19 +2133,19 @@
     </row>
     <row r="35" spans="1:22" ht="14.4">
       <c r="A35" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="15"/>
+        <v>42</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="13"/>
       <c r="D35" s="5">
-        <v>70661439</v>
+        <v>70629609</v>
       </c>
       <c r="E35" s="5">
-        <v>70665387</v>
-      </c>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
+        <v>70655281</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -2167,15 +2163,15 @@
     </row>
     <row r="36" spans="1:22" ht="14.4">
       <c r="A36" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="15"/>
       <c r="D36" s="5">
-        <v>70674326</v>
+        <v>70661439</v>
       </c>
       <c r="E36" s="5">
-        <v>70732345</v>
+        <v>70665387</v>
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
@@ -2197,19 +2193,19 @@
     </row>
     <row r="37" spans="1:22" ht="14.4">
       <c r="A37" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="13"/>
+        <v>44</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="15"/>
       <c r="D37" s="5">
-        <v>70692877</v>
+        <v>70674326</v>
       </c>
       <c r="E37" s="5">
-        <v>70693680</v>
-      </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
+        <v>70732345</v>
+      </c>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
@@ -2227,15 +2223,15 @@
     </row>
     <row r="38" spans="1:22" ht="14.4">
       <c r="A38" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="13"/>
       <c r="D38" s="5">
-        <v>70755013</v>
+        <v>70692877</v>
       </c>
       <c r="E38" s="5">
-        <v>70759135</v>
+        <v>70693680</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -2257,19 +2253,19 @@
     </row>
     <row r="39" spans="1:22" ht="14.4">
       <c r="A39" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="14"/>
+        <v>46</v>
+      </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="13"/>
       <c r="D39" s="5">
-        <v>70765125</v>
+        <v>70755013</v>
       </c>
       <c r="E39" s="5">
-        <v>70782692</v>
-      </c>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
+        <v>70759135</v>
+      </c>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
@@ -2287,15 +2283,15 @@
     </row>
     <row r="40" spans="1:22" ht="14.4">
       <c r="A40" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="16"/>
-      <c r="C40" s="15"/>
+      <c r="C40" s="14"/>
       <c r="D40" s="5">
-        <v>70784055</v>
+        <v>70765125</v>
       </c>
       <c r="E40" s="5">
-        <v>70790921</v>
+        <v>70782692</v>
       </c>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
@@ -2317,15 +2313,15 @@
     </row>
     <row r="41" spans="1:22" ht="14.4">
       <c r="A41" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="16"/>
-      <c r="C41" s="14"/>
+      <c r="C41" s="15"/>
       <c r="D41" s="5">
-        <v>70820545</v>
+        <v>70784055</v>
       </c>
       <c r="E41" s="5">
-        <v>70833184</v>
+        <v>70790921</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -2347,15 +2343,15 @@
     </row>
     <row r="42" spans="1:22" ht="14.4">
       <c r="A42" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B42" s="16"/>
-      <c r="C42" s="15"/>
+      <c r="C42" s="14"/>
       <c r="D42" s="5">
-        <v>70833297</v>
+        <v>70820545</v>
       </c>
       <c r="E42" s="5">
-        <v>70847080</v>
+        <v>70833184</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -2377,19 +2373,19 @@
     </row>
     <row r="43" spans="1:22" ht="14.4">
       <c r="A43" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="13"/>
+        <v>50</v>
+      </c>
+      <c r="B43" s="16"/>
+      <c r="C43" s="15"/>
       <c r="D43" s="5">
-        <v>70876934</v>
+        <v>70833297</v>
       </c>
       <c r="E43" s="5">
-        <v>70877235</v>
-      </c>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
+        <v>70847080</v>
+      </c>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
@@ -2407,19 +2403,19 @@
     </row>
     <row r="44" spans="1:22" ht="14.4">
       <c r="A44" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="15"/>
+        <v>51</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="13"/>
       <c r="D44" s="5">
-        <v>70890387</v>
+        <v>70876934</v>
       </c>
       <c r="E44" s="5">
-        <v>70916589</v>
-      </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
+        <v>70877235</v>
+      </c>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
@@ -2437,15 +2433,15 @@
     </row>
     <row r="45" spans="1:22" ht="14.4">
       <c r="A45" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" s="16"/>
       <c r="C45" s="15"/>
       <c r="D45" s="5">
-        <v>70953940</v>
+        <v>70890387</v>
       </c>
       <c r="E45" s="5">
-        <v>70960688</v>
+        <v>70916589</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -2467,15 +2463,15 @@
     </row>
     <row r="46" spans="1:22" ht="14.4">
       <c r="A46" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" s="16"/>
-      <c r="C46" s="14"/>
+      <c r="C46" s="15"/>
       <c r="D46" s="5">
-        <v>70957571</v>
+        <v>70953940</v>
       </c>
       <c r="E46" s="5">
-        <v>70985213</v>
+        <v>70960688</v>
       </c>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
@@ -2497,15 +2493,15 @@
     </row>
     <row r="47" spans="1:22" ht="14.4">
       <c r="A47" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B47" s="16"/>
-      <c r="C47" s="15"/>
+      <c r="C47" s="14"/>
       <c r="D47" s="5">
-        <v>70990569</v>
+        <v>70957571</v>
       </c>
       <c r="E47" s="5">
-        <v>71073583</v>
+        <v>70985213</v>
       </c>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
@@ -2527,19 +2523,19 @@
     </row>
     <row r="48" spans="1:22" ht="14.4">
       <c r="A48" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="13"/>
+        <v>55</v>
+      </c>
+      <c r="B48" s="16"/>
+      <c r="C48" s="15"/>
       <c r="D48" s="5">
-        <v>71071562</v>
+        <v>70990569</v>
       </c>
       <c r="E48" s="5">
-        <v>71085250</v>
-      </c>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
+        <v>71073583</v>
+      </c>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
@@ -2557,19 +2553,19 @@
     </row>
     <row r="49" spans="1:22" ht="14.4">
       <c r="A49" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B49" s="16"/>
-      <c r="C49" s="15"/>
+        <v>56</v>
+      </c>
+      <c r="B49" s="11"/>
+      <c r="C49" s="13"/>
       <c r="D49" s="5">
-        <v>71085339</v>
+        <v>71071562</v>
       </c>
       <c r="E49" s="5">
-        <v>71133963</v>
-      </c>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
+        <v>71085250</v>
+      </c>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -2587,15 +2583,15 @@
     </row>
     <row r="50" spans="1:22" ht="14.4">
       <c r="A50" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B50" s="16"/>
-      <c r="C50" s="14"/>
+      <c r="C50" s="15"/>
       <c r="D50" s="5">
-        <v>71133340</v>
+        <v>71085339</v>
       </c>
       <c r="E50" s="5">
-        <v>71140105</v>
+        <v>71133963</v>
       </c>
       <c r="F50" s="11"/>
       <c r="G50" s="11"/>
@@ -2617,15 +2613,15 @@
     </row>
     <row r="51" spans="1:22" ht="14.4">
       <c r="A51" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B51" s="16"/>
-      <c r="C51" s="15"/>
+      <c r="C51" s="14"/>
       <c r="D51" s="5">
-        <v>71144173</v>
+        <v>71133340</v>
       </c>
       <c r="E51" s="5">
-        <v>71175164</v>
+        <v>71140105</v>
       </c>
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
@@ -2647,19 +2643,19 @@
     </row>
     <row r="52" spans="1:22" ht="14.4">
       <c r="A52" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="13"/>
+        <v>59</v>
+      </c>
+      <c r="B52" s="16"/>
+      <c r="C52" s="15"/>
       <c r="D52" s="5">
-        <v>71169960</v>
+        <v>71144173</v>
       </c>
       <c r="E52" s="5">
-        <v>71171102</v>
-      </c>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
+        <v>71175164</v>
+      </c>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -2677,19 +2673,19 @@
     </row>
     <row r="53" spans="1:22" ht="14.4">
       <c r="A53" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B53" s="16"/>
-      <c r="C53" s="14"/>
+        <v>60</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="13"/>
       <c r="D53" s="5">
-        <v>71209817</v>
+        <v>71169960</v>
       </c>
       <c r="E53" s="5">
-        <v>71236775</v>
-      </c>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
+        <v>71171102</v>
+      </c>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -2707,15 +2703,15 @@
     </row>
     <row r="54" spans="1:22" ht="14.4">
       <c r="A54" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B54" s="16"/>
-      <c r="C54" s="15"/>
+      <c r="C54" s="14"/>
       <c r="D54" s="5">
-        <v>79336540</v>
+        <v>71209817</v>
       </c>
       <c r="E54" s="5">
-        <v>79340104</v>
+        <v>71236775</v>
       </c>
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
@@ -2737,15 +2733,15 @@
     </row>
     <row r="55" spans="1:22" ht="14.4">
       <c r="A55" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B55" s="16"/>
-      <c r="C55" s="14"/>
+      <c r="C55" s="15"/>
       <c r="D55" s="5">
-        <v>79362883</v>
+        <v>79336540</v>
       </c>
       <c r="E55" s="5">
-        <v>79364074</v>
+        <v>79340104</v>
       </c>
       <c r="F55" s="11"/>
       <c r="G55" s="11"/>
@@ -2767,15 +2763,15 @@
     </row>
     <row r="56" spans="1:22" ht="14.4">
       <c r="A56" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B56" s="16"/>
       <c r="C56" s="14"/>
       <c r="D56" s="5">
-        <v>79616839</v>
+        <v>79362883</v>
       </c>
       <c r="E56" s="5">
-        <v>79621245</v>
+        <v>79364074</v>
       </c>
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
@@ -2797,19 +2793,19 @@
     </row>
     <row r="57" spans="1:22" ht="14.4">
       <c r="A57" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B57" s="11"/>
-      <c r="C57" s="13"/>
+        <v>64</v>
+      </c>
+      <c r="B57" s="16"/>
+      <c r="C57" s="14"/>
       <c r="D57" s="5">
-        <v>79693141</v>
+        <v>79616839</v>
       </c>
       <c r="E57" s="5">
-        <v>79706102</v>
-      </c>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
+        <v>79621245</v>
+      </c>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
@@ -2827,19 +2823,19 @@
     </row>
     <row r="58" spans="1:22" ht="14.4">
       <c r="A58" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="B58" s="16"/>
-      <c r="C58" s="14"/>
+        <v>65</v>
+      </c>
+      <c r="B58" s="11"/>
+      <c r="C58" s="13"/>
       <c r="D58" s="5">
-        <v>79705788</v>
+        <v>79693141</v>
       </c>
       <c r="E58" s="5">
-        <v>79770724</v>
-      </c>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
+        <v>79706102</v>
+      </c>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
@@ -2857,15 +2853,15 @@
     </row>
     <row r="59" spans="1:22" ht="14.4">
       <c r="A59" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B59" s="16"/>
-      <c r="C59" s="15"/>
+      <c r="C59" s="14"/>
       <c r="D59" s="5">
-        <v>79780813</v>
+        <v>79705788</v>
       </c>
       <c r="E59" s="5">
-        <v>79784271</v>
+        <v>79770724</v>
       </c>
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
@@ -2887,19 +2883,19 @@
     </row>
     <row r="60" spans="1:22" ht="14.4">
       <c r="A60" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60" s="11"/>
-      <c r="C60" s="13"/>
+        <v>67</v>
+      </c>
+      <c r="B60" s="16"/>
+      <c r="C60" s="15"/>
       <c r="D60" s="5">
-        <v>79793501</v>
+        <v>79780813</v>
       </c>
       <c r="E60" s="5">
-        <v>79794371</v>
-      </c>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
+        <v>79784271</v>
+      </c>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
@@ -2917,19 +2913,19 @@
     </row>
     <row r="61" spans="1:22" ht="14.4">
       <c r="A61" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="B61" s="16"/>
-      <c r="C61" s="15"/>
+        <v>68</v>
+      </c>
+      <c r="B61" s="11"/>
+      <c r="C61" s="13"/>
       <c r="D61" s="5">
-        <v>79880646</v>
+        <v>79793501</v>
       </c>
       <c r="E61" s="5">
-        <v>80020253</v>
-      </c>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
+        <v>79794371</v>
+      </c>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
@@ -2947,19 +2943,19 @@
     </row>
     <row r="62" spans="1:22" ht="14.4">
       <c r="A62" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="B62" s="11"/>
-      <c r="C62" s="17"/>
+        <v>69</v>
+      </c>
+      <c r="B62" s="16"/>
+      <c r="C62" s="15"/>
       <c r="D62" s="5">
-        <v>80071036</v>
+        <v>79880646</v>
       </c>
       <c r="E62" s="5">
-        <v>80071108</v>
-      </c>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
+        <v>80020253</v>
+      </c>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
@@ -2977,19 +2973,19 @@
     </row>
     <row r="63" spans="1:22" ht="14.4">
       <c r="A63" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="B63" s="16"/>
-      <c r="C63" s="14"/>
+        <v>70</v>
+      </c>
+      <c r="B63" s="11"/>
+      <c r="C63" s="17"/>
       <c r="D63" s="5">
-        <v>80092745</v>
+        <v>80071036</v>
       </c>
       <c r="E63" s="5">
-        <v>80105787</v>
-      </c>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11"/>
+        <v>80071108</v>
+      </c>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
@@ -3007,15 +3003,15 @@
     </row>
     <row r="64" spans="1:22" ht="14.4">
       <c r="A64" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B64" s="16"/>
       <c r="C64" s="14"/>
       <c r="D64" s="5">
-        <v>80128438</v>
+        <v>80092745</v>
       </c>
       <c r="E64" s="5">
-        <v>80141956</v>
+        <v>80105787</v>
       </c>
       <c r="F64" s="11"/>
       <c r="G64" s="11"/>
@@ -3037,15 +3033,15 @@
     </row>
     <row r="65" spans="1:22" ht="14.4">
       <c r="A65" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B65" s="16"/>
       <c r="C65" s="14"/>
       <c r="D65" s="5">
-        <v>80141693</v>
+        <v>80128438</v>
       </c>
       <c r="E65" s="5">
-        <v>80148253</v>
+        <v>80141956</v>
       </c>
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
@@ -3067,15 +3063,15 @@
     </row>
     <row r="66" spans="1:22" ht="14.4">
       <c r="A66" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B66" s="16"/>
       <c r="C66" s="14"/>
       <c r="D66" s="5">
-        <v>80144820</v>
+        <v>80141693</v>
       </c>
       <c r="E66" s="5">
-        <v>80144924</v>
+        <v>80148253</v>
       </c>
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
@@ -3097,15 +3093,15 @@
     </row>
     <row r="67" spans="1:22" ht="14.4">
       <c r="A67" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B67" s="16"/>
       <c r="C67" s="14"/>
       <c r="D67" s="5">
-        <v>80175447</v>
+        <v>80144820</v>
       </c>
       <c r="E67" s="5">
-        <v>80201003</v>
+        <v>80144924</v>
       </c>
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
@@ -3127,15 +3123,15 @@
     </row>
     <row r="68" spans="1:22" ht="14.4">
       <c r="A68" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B68" s="16"/>
       <c r="C68" s="14"/>
       <c r="D68" s="5">
-        <v>80206861</v>
+        <v>80175447</v>
       </c>
       <c r="E68" s="5">
-        <v>80214843</v>
+        <v>80201003</v>
       </c>
       <c r="F68" s="11"/>
       <c r="G68" s="11"/>
@@ -3157,15 +3153,15 @@
     </row>
     <row r="69" spans="1:22" ht="14.4">
       <c r="A69" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B69" s="16"/>
       <c r="C69" s="14"/>
       <c r="D69" s="5">
-        <v>80226559</v>
+        <v>80206861</v>
       </c>
       <c r="E69" s="5">
-        <v>80241470</v>
+        <v>80214843</v>
       </c>
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
@@ -3187,15 +3183,15 @@
     </row>
     <row r="70" spans="1:22" ht="14.4">
       <c r="A70" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B70" s="16"/>
       <c r="C70" s="14"/>
       <c r="D70" s="5">
-        <v>80273479</v>
+        <v>80226559</v>
       </c>
       <c r="E70" s="5">
-        <v>80280715</v>
+        <v>80241470</v>
       </c>
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
@@ -3217,19 +3213,19 @@
     </row>
     <row r="71" spans="1:22" ht="14.4">
       <c r="A71" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B71" s="4"/>
-      <c r="C71" s="12"/>
+        <v>78</v>
+      </c>
+      <c r="B71" s="16"/>
+      <c r="C71" s="14"/>
       <c r="D71" s="5">
-        <v>80278213</v>
+        <v>80273479</v>
       </c>
       <c r="E71" s="5">
-        <v>80285131</v>
-      </c>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
+        <v>80280715</v>
+      </c>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
@@ -3247,19 +3243,19 @@
     </row>
     <row r="72" spans="1:22" ht="14.4">
       <c r="A72" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="B72" s="16"/>
-      <c r="C72" s="13"/>
+        <v>79</v>
+      </c>
+      <c r="B72" s="4"/>
+      <c r="C72" s="12"/>
       <c r="D72" s="5">
-        <v>80303639</v>
+        <v>80278213</v>
       </c>
       <c r="E72" s="5">
-        <v>80323058</v>
-      </c>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="11"/>
+        <v>80285131</v>
+      </c>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
@@ -3277,15 +3273,15 @@
     </row>
     <row r="73" spans="1:22" ht="14.4">
       <c r="A73" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B73" s="16"/>
-      <c r="C73" s="14"/>
+      <c r="C73" s="13"/>
       <c r="D73" s="5">
-        <v>80319786</v>
+        <v>80303639</v>
       </c>
       <c r="E73" s="5">
-        <v>80347985</v>
+        <v>80323058</v>
       </c>
       <c r="F73" s="11"/>
       <c r="G73" s="11"/>
@@ -3307,15 +3303,15 @@
     </row>
     <row r="74" spans="1:22" ht="14.4">
       <c r="A74" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B74" s="16"/>
-      <c r="C74" s="15"/>
+      <c r="C74" s="14"/>
       <c r="D74" s="5">
-        <v>80347993</v>
+        <v>80319786</v>
       </c>
       <c r="E74" s="5">
-        <v>80353625</v>
+        <v>80347985</v>
       </c>
       <c r="F74" s="11"/>
       <c r="G74" s="11"/>
@@ -3337,15 +3333,15 @@
     </row>
     <row r="75" spans="1:22" ht="14.4">
       <c r="A75" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B75" s="16"/>
-      <c r="C75" s="14"/>
+      <c r="C75" s="15"/>
       <c r="D75" s="5">
-        <v>80614152</v>
+        <v>80347993</v>
       </c>
       <c r="E75" s="5">
-        <v>80773626</v>
+        <v>80353625</v>
       </c>
       <c r="F75" s="11"/>
       <c r="G75" s="11"/>
@@ -3367,15 +3363,15 @@
     </row>
     <row r="76" spans="1:22" ht="14.4">
       <c r="A76" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B76" s="16"/>
       <c r="C76" s="14"/>
       <c r="D76" s="5">
-        <v>80808540</v>
+        <v>80614152</v>
       </c>
       <c r="E76" s="5">
-        <v>80865413</v>
+        <v>80773626</v>
       </c>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
@@ -3397,19 +3393,19 @@
     </row>
     <row r="77" spans="1:22" ht="14.4">
       <c r="A77" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="B77" s="4"/>
-      <c r="C77" s="18"/>
+        <v>84</v>
+      </c>
+      <c r="B77" s="16"/>
+      <c r="C77" s="14"/>
       <c r="D77" s="5">
-        <v>80926354</v>
+        <v>80808540</v>
       </c>
       <c r="E77" s="5">
-        <v>80947026</v>
-      </c>
-      <c r="F77" s="4"/>
-      <c r="G77" s="4"/>
-      <c r="H77" s="4"/>
+        <v>80865413</v>
+      </c>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
@@ -3427,15 +3423,15 @@
     </row>
     <row r="78" spans="1:22" ht="14.4">
       <c r="A78" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B78" s="4"/>
-      <c r="C78" s="12"/>
+      <c r="C78" s="18"/>
       <c r="D78" s="5">
-        <v>80963190</v>
+        <v>80926354</v>
       </c>
       <c r="E78" s="5">
-        <v>80977022</v>
+        <v>80947026</v>
       </c>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
@@ -3457,15 +3453,15 @@
     </row>
     <row r="79" spans="1:22" ht="14.4">
       <c r="A79" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="12"/>
       <c r="D79" s="5">
-        <v>80977471</v>
+        <v>80963190</v>
       </c>
       <c r="E79" s="5">
-        <v>80982370</v>
+        <v>80977022</v>
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
@@ -3487,19 +3483,19 @@
     </row>
     <row r="80" spans="1:22" ht="14.4">
       <c r="A80" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="B80" s="16"/>
-      <c r="C80" s="14"/>
+        <v>87</v>
+      </c>
+      <c r="B80" s="4"/>
+      <c r="C80" s="12"/>
       <c r="D80" s="5">
-        <v>81081005</v>
+        <v>80977471</v>
       </c>
       <c r="E80" s="5">
-        <v>81245002</v>
-      </c>
-      <c r="F80" s="11"/>
-      <c r="G80" s="11"/>
-      <c r="H80" s="11"/>
+        <v>80982370</v>
+      </c>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
@@ -3517,15 +3513,15 @@
     </row>
     <row r="81" spans="1:22" ht="14.4">
       <c r="A81" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B81" s="16"/>
       <c r="C81" s="14"/>
       <c r="D81" s="5">
-        <v>81240819</v>
+        <v>81081005</v>
       </c>
       <c r="E81" s="5">
-        <v>81293201</v>
+        <v>81245002</v>
       </c>
       <c r="F81" s="11"/>
       <c r="G81" s="11"/>
@@ -3547,15 +3543,15 @@
     </row>
     <row r="82" spans="1:22" ht="14.4">
       <c r="A82" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B82" s="16"/>
       <c r="C82" s="14"/>
       <c r="D82" s="5">
-        <v>82506638</v>
+        <v>81240819</v>
       </c>
       <c r="E82" s="5">
-        <v>82511053</v>
+        <v>81293201</v>
       </c>
       <c r="F82" s="11"/>
       <c r="G82" s="11"/>
@@ -3577,15 +3573,15 @@
     </row>
     <row r="83" spans="1:22" ht="14.4">
       <c r="A83" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B83" s="16"/>
-      <c r="C83" s="15"/>
+      <c r="C83" s="14"/>
       <c r="D83" s="5">
-        <v>82511212</v>
+        <v>82506638</v>
       </c>
       <c r="E83" s="5">
-        <v>82526061</v>
+        <v>82511053</v>
       </c>
       <c r="F83" s="11"/>
       <c r="G83" s="11"/>
@@ -3607,19 +3603,19 @@
     </row>
     <row r="84" spans="1:22" ht="14.4">
       <c r="A84" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="B84" s="4"/>
-      <c r="C84" s="12"/>
+        <v>91</v>
+      </c>
+      <c r="B84" s="16"/>
+      <c r="C84" s="15"/>
       <c r="D84" s="5">
-        <v>82515882</v>
+        <v>82511212</v>
       </c>
       <c r="E84" s="5">
-        <v>82516400</v>
-      </c>
-      <c r="F84" s="4"/>
-      <c r="G84" s="4"/>
-      <c r="H84" s="4"/>
+        <v>82526061</v>
+      </c>
+      <c r="F84" s="11"/>
+      <c r="G84" s="11"/>
+      <c r="H84" s="11"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
@@ -3637,19 +3633,19 @@
     </row>
     <row r="85" spans="1:22" ht="14.4">
       <c r="A85" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="B85" s="16"/>
-      <c r="C85" s="14"/>
+        <v>92</v>
+      </c>
+      <c r="B85" s="4"/>
+      <c r="C85" s="12"/>
       <c r="D85" s="5">
-        <v>82525974</v>
+        <v>82515882</v>
       </c>
       <c r="E85" s="5">
-        <v>82535295</v>
-      </c>
-      <c r="F85" s="11"/>
-      <c r="G85" s="11"/>
-      <c r="H85" s="11"/>
+        <v>82516400</v>
+      </c>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
+      <c r="H85" s="4"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
@@ -3667,15 +3663,15 @@
     </row>
     <row r="86" spans="1:22" ht="14.4">
       <c r="A86" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B86" s="16"/>
       <c r="C86" s="14"/>
       <c r="D86" s="5">
-        <v>82535406</v>
+        <v>82525974</v>
       </c>
       <c r="E86" s="5">
-        <v>82554352</v>
+        <v>82535295</v>
       </c>
       <c r="F86" s="11"/>
       <c r="G86" s="11"/>
@@ -3697,15 +3693,15 @@
     </row>
     <row r="87" spans="1:22" ht="14.4">
       <c r="A87" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B87" s="16"/>
       <c r="C87" s="14"/>
       <c r="D87" s="5">
-        <v>82560802</v>
+        <v>82535406</v>
       </c>
       <c r="E87" s="5">
-        <v>82569668</v>
+        <v>82554352</v>
       </c>
       <c r="F87" s="11"/>
       <c r="G87" s="11"/>
@@ -3727,15 +3723,15 @@
     </row>
     <row r="88" spans="1:22" ht="14.4">
       <c r="A88" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B88" s="16"/>
       <c r="C88" s="14"/>
       <c r="D88" s="5">
-        <v>82571368</v>
+        <v>82560802</v>
       </c>
       <c r="E88" s="5">
-        <v>82607245</v>
+        <v>82569668</v>
       </c>
       <c r="F88" s="11"/>
       <c r="G88" s="11"/>
@@ -3757,15 +3753,15 @@
     </row>
     <row r="89" spans="1:22" ht="14.4">
       <c r="A89" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B89" s="16"/>
       <c r="C89" s="14"/>
       <c r="D89" s="5">
-        <v>82598307</v>
+        <v>82571368</v>
       </c>
       <c r="E89" s="5">
-        <v>82600577</v>
+        <v>82607245</v>
       </c>
       <c r="F89" s="11"/>
       <c r="G89" s="11"/>
@@ -3787,15 +3783,15 @@
     </row>
     <row r="90" spans="1:22" ht="14.4">
       <c r="A90" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B90" s="16"/>
       <c r="C90" s="14"/>
       <c r="D90" s="5">
-        <v>82608065</v>
+        <v>82598307</v>
       </c>
       <c r="E90" s="5">
-        <v>82613537</v>
+        <v>82600577</v>
       </c>
       <c r="F90" s="11"/>
       <c r="G90" s="11"/>
@@ -3817,15 +3813,15 @@
     </row>
     <row r="91" spans="1:22" ht="14.4">
       <c r="A91" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B91" s="16"/>
       <c r="C91" s="14"/>
       <c r="D91" s="5">
-        <v>82614361</v>
+        <v>82608065</v>
       </c>
       <c r="E91" s="5">
-        <v>82614464</v>
+        <v>82613537</v>
       </c>
       <c r="F91" s="11"/>
       <c r="G91" s="11"/>
@@ -3847,15 +3843,15 @@
     </row>
     <row r="92" spans="1:22" ht="14.4">
       <c r="A92" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B92" s="16"/>
       <c r="C92" s="14"/>
       <c r="D92" s="5">
-        <v>82642969</v>
+        <v>82614361</v>
       </c>
       <c r="E92" s="5">
-        <v>82651231</v>
+        <v>82614464</v>
       </c>
       <c r="F92" s="11"/>
       <c r="G92" s="11"/>
@@ -3877,15 +3873,15 @@
     </row>
     <row r="93" spans="1:22" ht="14.4">
       <c r="A93" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B93" s="16"/>
       <c r="C93" s="14"/>
       <c r="D93" s="5">
-        <v>82653120</v>
+        <v>82642969</v>
       </c>
       <c r="E93" s="5">
-        <v>82662185</v>
+        <v>82651231</v>
       </c>
       <c r="F93" s="11"/>
       <c r="G93" s="11"/>
@@ -3907,15 +3903,15 @@
     </row>
     <row r="94" spans="1:22" ht="14.4">
       <c r="A94" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B94" s="16"/>
       <c r="C94" s="14"/>
       <c r="D94" s="5">
-        <v>82663789</v>
+        <v>82653120</v>
       </c>
       <c r="E94" s="5">
-        <v>82679754</v>
+        <v>82662185</v>
       </c>
       <c r="F94" s="11"/>
       <c r="G94" s="11"/>
@@ -3937,15 +3933,15 @@
     </row>
     <row r="95" spans="1:22" ht="14.4">
       <c r="A95" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B95" s="16"/>
-      <c r="C95" s="15"/>
+      <c r="C95" s="14"/>
       <c r="D95" s="5">
-        <v>82685406</v>
+        <v>82663789</v>
       </c>
       <c r="E95" s="5">
-        <v>82694696</v>
+        <v>82679754</v>
       </c>
       <c r="F95" s="11"/>
       <c r="G95" s="11"/>
@@ -3967,19 +3963,19 @@
     </row>
     <row r="96" spans="1:22" ht="14.4">
       <c r="A96" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="B96" s="4"/>
-      <c r="C96" s="18"/>
+        <v>103</v>
+      </c>
+      <c r="B96" s="16"/>
+      <c r="C96" s="15"/>
       <c r="D96" s="5">
-        <v>82714916</v>
+        <v>82685406</v>
       </c>
       <c r="E96" s="5">
-        <v>82721551</v>
+        <v>82694696</v>
       </c>
       <c r="F96" s="11"/>
-      <c r="G96" s="4"/>
-      <c r="H96" s="4"/>
+      <c r="G96" s="11"/>
+      <c r="H96" s="11"/>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
@@ -3997,17 +3993,17 @@
     </row>
     <row r="97" spans="1:22" ht="14.4">
       <c r="A97" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="18"/>
       <c r="D97" s="5">
-        <v>82744547</v>
+        <v>82714916</v>
       </c>
       <c r="E97" s="5">
-        <v>82751626</v>
-      </c>
-      <c r="F97" s="4"/>
+        <v>82721551</v>
+      </c>
+      <c r="F97" s="11"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="2"/>
@@ -4027,15 +4023,15 @@
     </row>
     <row r="98" spans="1:22" ht="14.4">
       <c r="A98" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B98" s="4"/>
-      <c r="C98" s="17"/>
+      <c r="C98" s="18"/>
       <c r="D98" s="5">
-        <v>82770624</v>
+        <v>82744547</v>
       </c>
       <c r="E98" s="5">
-        <v>82776005</v>
+        <v>82751626</v>
       </c>
       <c r="F98" s="4"/>
       <c r="G98" s="4"/>
@@ -4057,15 +4053,15 @@
     </row>
     <row r="99" spans="1:22" ht="14.4">
       <c r="A99" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="17"/>
       <c r="D99" s="5">
-        <v>82780306</v>
+        <v>82770624</v>
       </c>
       <c r="E99" s="5">
-        <v>82781320</v>
+        <v>82776005</v>
       </c>
       <c r="F99" s="4"/>
       <c r="G99" s="4"/>
@@ -4087,15 +4083,15 @@
     </row>
     <row r="100" spans="1:22" ht="14.4">
       <c r="A100" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="17"/>
       <c r="D100" s="5">
-        <v>82792580</v>
+        <v>82780306</v>
       </c>
       <c r="E100" s="5">
-        <v>82811159</v>
+        <v>82781320</v>
       </c>
       <c r="F100" s="4"/>
       <c r="G100" s="4"/>
@@ -4117,19 +4113,19 @@
     </row>
     <row r="101" spans="1:22" ht="14.4">
       <c r="A101" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="B101" s="16"/>
-      <c r="C101" s="14"/>
+        <v>108</v>
+      </c>
+      <c r="B101" s="4"/>
+      <c r="C101" s="17"/>
       <c r="D101" s="5">
-        <v>82810850</v>
+        <v>82792580</v>
       </c>
       <c r="E101" s="5">
-        <v>82893600</v>
-      </c>
-      <c r="F101" s="11"/>
-      <c r="G101" s="11"/>
-      <c r="H101" s="11"/>
+        <v>82811159</v>
+      </c>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
@@ -4147,19 +4143,19 @@
     </row>
     <row r="102" spans="1:22" ht="14.4">
       <c r="A102" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="B102" s="4"/>
-      <c r="C102" s="17"/>
+        <v>109</v>
+      </c>
+      <c r="B102" s="16"/>
+      <c r="C102" s="14"/>
       <c r="D102" s="5">
-        <v>82910365</v>
+        <v>82810850</v>
       </c>
       <c r="E102" s="5">
-        <v>82920081</v>
-      </c>
-      <c r="F102" s="4"/>
-      <c r="G102" s="4"/>
-      <c r="H102" s="4"/>
+        <v>82893600</v>
+      </c>
+      <c r="F102" s="11"/>
+      <c r="G102" s="11"/>
+      <c r="H102" s="11"/>
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
@@ -4177,19 +4173,19 @@
     </row>
     <row r="103" spans="1:22" ht="14.4">
       <c r="A103" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="B103" s="16"/>
-      <c r="C103" s="15"/>
+        <v>110</v>
+      </c>
+      <c r="B103" s="4"/>
+      <c r="C103" s="17"/>
       <c r="D103" s="5">
-        <v>82931563</v>
+        <v>82910365</v>
       </c>
       <c r="E103" s="5">
-        <v>82985019</v>
-      </c>
-      <c r="F103" s="11"/>
-      <c r="G103" s="11"/>
-      <c r="H103" s="11"/>
+        <v>82920081</v>
+      </c>
+      <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
+      <c r="H103" s="4"/>
       <c r="I103" s="2"/>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
@@ -4207,15 +4203,15 @@
     </row>
     <row r="104" spans="1:22" ht="14.4">
       <c r="A104" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B104" s="16"/>
-      <c r="C104" s="19"/>
+      <c r="C104" s="15"/>
       <c r="D104" s="5">
-        <v>82988294</v>
+        <v>82931563</v>
       </c>
       <c r="E104" s="5">
-        <v>82995755</v>
+        <v>82985019</v>
       </c>
       <c r="F104" s="11"/>
       <c r="G104" s="11"/>
@@ -4237,15 +4233,15 @@
     </row>
     <row r="105" spans="1:22" ht="14.4">
       <c r="A105" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B105" s="16"/>
-      <c r="C105" s="15"/>
+      <c r="C105" s="19"/>
       <c r="D105" s="5">
-        <v>82997831</v>
+        <v>82988294</v>
       </c>
       <c r="E105" s="5">
-        <v>83104794</v>
+        <v>82995755</v>
       </c>
       <c r="F105" s="11"/>
       <c r="G105" s="11"/>
@@ -4267,19 +4263,19 @@
     </row>
     <row r="106" spans="1:22" ht="14.4">
       <c r="A106" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="B106" s="4"/>
-      <c r="C106" s="17"/>
+        <v>113</v>
+      </c>
+      <c r="B106" s="16"/>
+      <c r="C106" s="15"/>
       <c r="D106" s="5">
-        <v>83057549</v>
+        <v>82997831</v>
       </c>
       <c r="E106" s="5">
-        <v>83058102</v>
-      </c>
-      <c r="F106" s="4"/>
-      <c r="G106" s="4"/>
-      <c r="H106" s="4"/>
+        <v>83104794</v>
+      </c>
+      <c r="F106" s="11"/>
+      <c r="G106" s="11"/>
+      <c r="H106" s="11"/>
       <c r="I106" s="2"/>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
@@ -4297,19 +4293,19 @@
     </row>
     <row r="107" spans="1:22" ht="14.4">
       <c r="A107" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="B107" s="16"/>
-      <c r="C107" s="15"/>
+        <v>114</v>
+      </c>
+      <c r="B107" s="4"/>
+      <c r="C107" s="17"/>
       <c r="D107" s="5">
-        <v>83132206</v>
+        <v>83057549</v>
       </c>
       <c r="E107" s="5">
-        <v>83168823</v>
-      </c>
-      <c r="F107" s="11"/>
-      <c r="G107" s="11"/>
-      <c r="H107" s="11"/>
+        <v>83058102</v>
+      </c>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+      <c r="H107" s="4"/>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
@@ -4327,19 +4323,19 @@
     </row>
     <row r="108" spans="1:22" ht="14.4">
       <c r="A108" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="B108" s="4"/>
-      <c r="C108" s="17"/>
+        <v>115</v>
+      </c>
+      <c r="B108" s="16"/>
+      <c r="C108" s="15"/>
       <c r="D108" s="5">
-        <v>83227637</v>
+        <v>83132206</v>
       </c>
       <c r="E108" s="5">
-        <v>83232424</v>
-      </c>
-      <c r="F108" s="4"/>
-      <c r="G108" s="4"/>
-      <c r="H108" s="4"/>
+        <v>83168823</v>
+      </c>
+      <c r="F108" s="11"/>
+      <c r="G108" s="11"/>
+      <c r="H108" s="11"/>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
@@ -4357,19 +4353,19 @@
     </row>
     <row r="109" spans="1:22" ht="14.4">
       <c r="A109" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="B109" s="16"/>
-      <c r="C109" s="14"/>
+        <v>116</v>
+      </c>
+      <c r="B109" s="4"/>
+      <c r="C109" s="17"/>
       <c r="D109" s="5">
-        <v>83232769</v>
+        <v>83227637</v>
       </c>
       <c r="E109" s="5">
-        <v>83289469</v>
-      </c>
-      <c r="F109" s="11"/>
-      <c r="G109" s="11"/>
-      <c r="H109" s="11"/>
+        <v>83232424</v>
+      </c>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="4"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
@@ -4387,19 +4383,19 @@
     </row>
     <row r="110" spans="1:22" ht="14.4">
       <c r="A110" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="B110" s="4"/>
-      <c r="C110" s="17"/>
+        <v>117</v>
+      </c>
+      <c r="B110" s="16"/>
+      <c r="C110" s="14"/>
       <c r="D110" s="5">
-        <v>83319445</v>
+        <v>83232769</v>
       </c>
       <c r="E110" s="5">
-        <v>83327074</v>
-      </c>
-      <c r="F110" s="4"/>
-      <c r="G110" s="4"/>
-      <c r="H110" s="4"/>
+        <v>83289469</v>
+      </c>
+      <c r="F110" s="11"/>
+      <c r="G110" s="11"/>
+      <c r="H110" s="11"/>
       <c r="I110" s="2"/>
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
@@ -4417,19 +4413,19 @@
     </row>
     <row r="111" spans="1:22" ht="14.4">
       <c r="A111" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B111" s="16"/>
-      <c r="C111" s="15"/>
+        <v>118</v>
+      </c>
+      <c r="B111" s="4"/>
+      <c r="C111" s="17"/>
       <c r="D111" s="5">
-        <v>83333199</v>
+        <v>83319445</v>
       </c>
       <c r="E111" s="5">
-        <v>83613814</v>
-      </c>
-      <c r="F111" s="11"/>
-      <c r="G111" s="11"/>
-      <c r="H111" s="11"/>
+        <v>83327074</v>
+      </c>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
+      <c r="H111" s="4"/>
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
@@ -4447,19 +4443,19 @@
     </row>
     <row r="112" spans="1:22" ht="14.4">
       <c r="A112" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="B112" s="4"/>
-      <c r="C112" s="17"/>
+        <v>119</v>
+      </c>
+      <c r="B112" s="16"/>
+      <c r="C112" s="15"/>
       <c r="D112" s="5">
-        <v>83445029</v>
+        <v>83333199</v>
       </c>
       <c r="E112" s="5">
-        <v>83452107</v>
-      </c>
-      <c r="F112" s="4"/>
-      <c r="G112" s="4"/>
-      <c r="H112" s="4"/>
+        <v>83613814</v>
+      </c>
+      <c r="F112" s="11"/>
+      <c r="G112" s="11"/>
+      <c r="H112" s="11"/>
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
@@ -4477,15 +4473,15 @@
     </row>
     <row r="113" spans="1:22" ht="14.4">
       <c r="A113" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B113" s="4"/>
       <c r="C113" s="17"/>
       <c r="D113" s="5">
-        <v>83487202</v>
+        <v>83445029</v>
       </c>
       <c r="E113" s="5">
-        <v>83492180</v>
+        <v>83452107</v>
       </c>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
@@ -4507,19 +4503,19 @@
     </row>
     <row r="114" spans="1:22" ht="14.4">
       <c r="A114" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="B114" s="16"/>
-      <c r="C114" s="14"/>
+        <v>121</v>
+      </c>
+      <c r="B114" s="4"/>
+      <c r="C114" s="17"/>
       <c r="D114" s="5">
-        <v>83504908</v>
+        <v>83487202</v>
       </c>
       <c r="E114" s="5">
-        <v>83522015</v>
-      </c>
-      <c r="F114" s="11"/>
-      <c r="G114" s="11"/>
-      <c r="H114" s="11"/>
+        <v>83492180</v>
+      </c>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+      <c r="H114" s="4"/>
       <c r="I114" s="2"/>
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
@@ -4537,19 +4533,19 @@
     </row>
     <row r="115" spans="1:22" ht="14.4">
       <c r="A115" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="B115" s="4"/>
-      <c r="C115" s="17"/>
+        <v>122</v>
+      </c>
+      <c r="B115" s="16"/>
+      <c r="C115" s="14"/>
       <c r="D115" s="5">
-        <v>83620763</v>
+        <v>83504908</v>
       </c>
       <c r="E115" s="5">
-        <v>83621974</v>
-      </c>
-      <c r="F115" s="4"/>
-      <c r="G115" s="4"/>
-      <c r="H115" s="4"/>
+        <v>83522015</v>
+      </c>
+      <c r="F115" s="11"/>
+      <c r="G115" s="11"/>
+      <c r="H115" s="11"/>
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
@@ -4567,19 +4563,19 @@
     </row>
     <row r="116" spans="1:22" ht="14.4">
       <c r="A116" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="B116" s="16"/>
-      <c r="C116" s="13"/>
+        <v>123</v>
+      </c>
+      <c r="B116" s="4"/>
+      <c r="C116" s="17"/>
       <c r="D116" s="5">
-        <v>83625794</v>
+        <v>83620763</v>
       </c>
       <c r="E116" s="5">
-        <v>83658751</v>
-      </c>
-      <c r="F116" s="11"/>
-      <c r="G116" s="11"/>
-      <c r="H116" s="11"/>
+        <v>83621974</v>
+      </c>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
+      <c r="H116" s="4"/>
       <c r="I116" s="2"/>
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
@@ -4597,15 +4593,15 @@
     </row>
     <row r="117" spans="1:22" ht="14.4">
       <c r="A117" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B117" s="16"/>
-      <c r="C117" s="14"/>
+      <c r="C117" s="13"/>
       <c r="D117" s="5">
-        <v>83672472</v>
+        <v>83625794</v>
       </c>
       <c r="E117" s="5">
-        <v>83725774</v>
+        <v>83658751</v>
       </c>
       <c r="F117" s="11"/>
       <c r="G117" s="11"/>
@@ -4627,15 +4623,15 @@
     </row>
     <row r="118" spans="1:22" ht="14.4">
       <c r="A118" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B118" s="16"/>
       <c r="C118" s="14"/>
       <c r="D118" s="5">
-        <v>83751836</v>
+        <v>83672472</v>
       </c>
       <c r="E118" s="5">
-        <v>83782623</v>
+        <v>83725774</v>
       </c>
       <c r="F118" s="11"/>
       <c r="G118" s="11"/>
@@ -4657,15 +4653,15 @@
     </row>
     <row r="119" spans="1:22" ht="14.4">
       <c r="A119" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B119" s="16"/>
-      <c r="C119" s="15"/>
+      <c r="C119" s="14"/>
       <c r="D119" s="5">
-        <v>83809139</v>
+        <v>83751836</v>
       </c>
       <c r="E119" s="5">
-        <v>83921211</v>
+        <v>83782623</v>
       </c>
       <c r="F119" s="11"/>
       <c r="G119" s="11"/>
@@ -4687,19 +4683,19 @@
     </row>
     <row r="120" spans="1:22" ht="14.4">
       <c r="A120" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B120" s="4"/>
-      <c r="C120" s="17"/>
+        <v>127</v>
+      </c>
+      <c r="B120" s="16"/>
+      <c r="C120" s="15"/>
       <c r="D120" s="5">
-        <v>83998316</v>
+        <v>83809139</v>
       </c>
       <c r="E120" s="5">
-        <v>83998387</v>
-      </c>
-      <c r="F120" s="4"/>
-      <c r="G120" s="4"/>
-      <c r="H120" s="4"/>
+        <v>83921211</v>
+      </c>
+      <c r="F120" s="11"/>
+      <c r="G120" s="11"/>
+      <c r="H120" s="11"/>
       <c r="I120" s="2"/>
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
@@ -4717,15 +4713,15 @@
     </row>
     <row r="121" spans="1:22" ht="14.4">
       <c r="A121" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="B121" s="20"/>
-      <c r="C121" s="20"/>
+        <v>10</v>
+      </c>
+      <c r="B121" s="4"/>
+      <c r="C121" s="17"/>
       <c r="D121" s="5">
-        <v>95470430</v>
+        <v>83998316</v>
       </c>
       <c r="E121" s="5">
-        <v>95581144</v>
+        <v>83998387</v>
       </c>
       <c r="F121" s="4"/>
       <c r="G121" s="4"/>
@@ -4747,19 +4743,19 @@
     </row>
     <row r="122" spans="1:22" ht="14.4">
       <c r="A122" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="B122" s="16"/>
-      <c r="C122" s="14"/>
+        <v>128</v>
+      </c>
+      <c r="B122" s="20"/>
+      <c r="C122" s="20"/>
       <c r="D122" s="5">
-        <v>95581209</v>
+        <v>95470430</v>
       </c>
       <c r="E122" s="5">
-        <v>95978163</v>
-      </c>
-      <c r="F122" s="11"/>
-      <c r="G122" s="11"/>
-      <c r="H122" s="11"/>
+        <v>95581144</v>
+      </c>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+      <c r="H122" s="4"/>
       <c r="I122" s="2"/>
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
@@ -4777,15 +4773,15 @@
     </row>
     <row r="123" spans="1:22" ht="14.4">
       <c r="A123" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B123" s="16"/>
       <c r="C123" s="14"/>
       <c r="D123" s="5">
-        <v>96002983</v>
+        <v>95581209</v>
       </c>
       <c r="E123" s="5">
-        <v>96037965</v>
+        <v>95978163</v>
       </c>
       <c r="F123" s="11"/>
       <c r="G123" s="11"/>
@@ -4807,19 +4803,19 @@
     </row>
     <row r="124" spans="1:22" ht="14.4">
       <c r="A124" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="B124" s="11"/>
-      <c r="C124" s="20"/>
+        <v>130</v>
+      </c>
+      <c r="B124" s="16"/>
+      <c r="C124" s="14"/>
       <c r="D124" s="5">
-        <v>96059361</v>
+        <v>96002983</v>
       </c>
       <c r="E124" s="5">
-        <v>96082527</v>
-      </c>
-      <c r="F124" s="4"/>
-      <c r="G124" s="4"/>
-      <c r="H124" s="4"/>
+        <v>96037965</v>
+      </c>
+      <c r="F124" s="11"/>
+      <c r="G124" s="11"/>
+      <c r="H124" s="11"/>
       <c r="I124" s="2"/>
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
@@ -4837,19 +4833,19 @@
     </row>
     <row r="125" spans="1:22" ht="14.4">
       <c r="A125" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="B125" s="16"/>
-      <c r="C125" s="15"/>
+        <v>131</v>
+      </c>
+      <c r="B125" s="11"/>
+      <c r="C125" s="20"/>
       <c r="D125" s="5">
-        <v>96089557</v>
+        <v>96059361</v>
       </c>
       <c r="E125" s="5">
-        <v>96111990</v>
-      </c>
-      <c r="F125" s="11"/>
-      <c r="G125" s="11"/>
-      <c r="H125" s="11"/>
+        <v>96082527</v>
+      </c>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
+      <c r="H125" s="4"/>
       <c r="I125" s="2"/>
       <c r="J125" s="2"/>
       <c r="K125" s="2"/>
@@ -4867,15 +4863,15 @@
     </row>
     <row r="126" spans="1:22" ht="14.4">
       <c r="A126" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B126" s="16"/>
-      <c r="C126" s="14"/>
+      <c r="C126" s="15"/>
       <c r="D126" s="5">
-        <v>96121289</v>
+        <v>96089557</v>
       </c>
       <c r="E126" s="5">
-        <v>96125042</v>
+        <v>96111990</v>
       </c>
       <c r="F126" s="11"/>
       <c r="G126" s="11"/>
@@ -4897,15 +4893,15 @@
     </row>
     <row r="127" spans="1:22" ht="14.4">
       <c r="A127" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B127" s="16"/>
       <c r="C127" s="14"/>
       <c r="D127" s="5">
-        <v>96402759</v>
+        <v>96121289</v>
       </c>
       <c r="E127" s="5">
-        <v>96518138</v>
+        <v>96125042</v>
       </c>
       <c r="F127" s="11"/>
       <c r="G127" s="11"/>
@@ -4927,15 +4923,15 @@
     </row>
     <row r="128" spans="1:22" ht="14.4">
       <c r="A128" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B128" s="16"/>
       <c r="C128" s="14"/>
       <c r="D128" s="5">
-        <v>96537063</v>
+        <v>96402759</v>
       </c>
       <c r="E128" s="5">
-        <v>96551940</v>
+        <v>96518138</v>
       </c>
       <c r="F128" s="11"/>
       <c r="G128" s="11"/>
@@ -4957,15 +4953,15 @@
     </row>
     <row r="129" spans="1:22" ht="14.4">
       <c r="A129" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B129" s="16"/>
       <c r="C129" s="14"/>
       <c r="D129" s="5">
-        <v>96570613</v>
+        <v>96537063</v>
       </c>
       <c r="E129" s="5">
-        <v>96599056</v>
+        <v>96551940</v>
       </c>
       <c r="F129" s="11"/>
       <c r="G129" s="11"/>
@@ -4987,15 +4983,15 @@
     </row>
     <row r="130" spans="1:22" ht="14.4">
       <c r="A130" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B130" s="16"/>
       <c r="C130" s="14"/>
       <c r="D130" s="5">
-        <v>96633813</v>
+        <v>96570613</v>
       </c>
       <c r="E130" s="5">
-        <v>96703313</v>
+        <v>96599056</v>
       </c>
       <c r="F130" s="11"/>
       <c r="G130" s="11"/>
@@ -5017,15 +5013,15 @@
     </row>
     <row r="131" spans="1:22" ht="14.4">
       <c r="A131" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B131" s="16"/>
       <c r="C131" s="14"/>
       <c r="D131" s="5">
-        <v>96736216</v>
+        <v>96633813</v>
       </c>
       <c r="E131" s="5">
-        <v>96809367</v>
+        <v>96703313</v>
       </c>
       <c r="F131" s="11"/>
       <c r="G131" s="11"/>
@@ -5047,19 +5043,19 @@
     </row>
     <row r="132" spans="1:22" ht="14.4">
       <c r="A132" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="B132" s="1"/>
-      <c r="C132" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="B132" s="16"/>
+      <c r="C132" s="14"/>
       <c r="D132" s="5">
-        <v>96782525</v>
+        <v>96736216</v>
       </c>
       <c r="E132" s="5">
-        <v>96786132</v>
-      </c>
-      <c r="F132" s="4"/>
-      <c r="G132" s="4"/>
-      <c r="H132" s="4"/>
+        <v>96809367</v>
+      </c>
+      <c r="F132" s="11"/>
+      <c r="G132" s="11"/>
+      <c r="H132" s="11"/>
       <c r="I132" s="2"/>
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
@@ -5077,19 +5073,19 @@
     </row>
     <row r="133" spans="1:22" ht="14.4">
       <c r="A133" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="B133" s="16"/>
-      <c r="C133" s="14"/>
+        <v>139</v>
+      </c>
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
       <c r="D133" s="5">
-        <v>96816926</v>
+        <v>96782525</v>
       </c>
       <c r="E133" s="5">
-        <v>96881009</v>
-      </c>
-      <c r="F133" s="11"/>
-      <c r="G133" s="11"/>
-      <c r="H133" s="11"/>
+        <v>96786132</v>
+      </c>
+      <c r="F133" s="4"/>
+      <c r="G133" s="4"/>
+      <c r="H133" s="4"/>
       <c r="I133" s="2"/>
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
@@ -5107,19 +5103,19 @@
     </row>
     <row r="134" spans="1:22" ht="14.4">
       <c r="A134" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="B134" s="1"/>
-      <c r="C134" s="1"/>
+        <v>140</v>
+      </c>
+      <c r="B134" s="16"/>
+      <c r="C134" s="14"/>
       <c r="D134" s="5">
-        <v>96872046</v>
+        <v>96816926</v>
       </c>
       <c r="E134" s="5">
-        <v>96873477</v>
-      </c>
-      <c r="F134" s="4"/>
-      <c r="G134" s="4"/>
-      <c r="H134" s="4"/>
+        <v>96881009</v>
+      </c>
+      <c r="F134" s="11"/>
+      <c r="G134" s="11"/>
+      <c r="H134" s="11"/>
       <c r="I134" s="2"/>
       <c r="J134" s="2"/>
       <c r="K134" s="2"/>
@@ -5137,15 +5133,15 @@
     </row>
     <row r="135" spans="1:22" ht="14.4">
       <c r="A135" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="B135" s="11"/>
+        <v>141</v>
+      </c>
+      <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="5">
-        <v>96905989</v>
+        <v>96872046</v>
       </c>
       <c r="E135" s="5">
-        <v>96906172</v>
+        <v>96873477</v>
       </c>
       <c r="F135" s="4"/>
       <c r="G135" s="4"/>
@@ -5167,19 +5163,19 @@
     </row>
     <row r="136" spans="1:22" ht="14.4">
       <c r="A136" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="B136" s="16"/>
-      <c r="C136" s="14"/>
+        <v>142</v>
+      </c>
+      <c r="B136" s="11"/>
+      <c r="C136" s="1"/>
       <c r="D136" s="5">
-        <v>96913066</v>
+        <v>96905989</v>
       </c>
       <c r="E136" s="5">
-        <v>96946841</v>
-      </c>
-      <c r="F136" s="11"/>
-      <c r="G136" s="11"/>
-      <c r="H136" s="11"/>
+        <v>96906172</v>
+      </c>
+      <c r="F136" s="4"/>
+      <c r="G136" s="4"/>
+      <c r="H136" s="4"/>
       <c r="I136" s="2"/>
       <c r="J136" s="2"/>
       <c r="K136" s="2"/>
@@ -5197,15 +5193,15 @@
     </row>
     <row r="137" spans="1:22" ht="14.4">
       <c r="A137" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B137" s="16"/>
       <c r="C137" s="14"/>
       <c r="D137" s="5">
-        <v>96967164</v>
+        <v>96913066</v>
       </c>
       <c r="E137" s="5">
-        <v>96982920</v>
+        <v>96946841</v>
       </c>
       <c r="F137" s="11"/>
       <c r="G137" s="11"/>
@@ -5227,15 +5223,15 @@
     </row>
     <row r="138" spans="1:22" ht="14.4">
       <c r="A138" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B138" s="16"/>
       <c r="C138" s="14"/>
       <c r="D138" s="5">
-        <v>97036910</v>
+        <v>96967164</v>
       </c>
       <c r="E138" s="5">
-        <v>97064068</v>
+        <v>96982920</v>
       </c>
       <c r="F138" s="11"/>
       <c r="G138" s="11"/>
@@ -5257,15 +5253,15 @@
     </row>
     <row r="139" spans="1:22" ht="14.4">
       <c r="A139" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B139" s="16"/>
       <c r="C139" s="14"/>
       <c r="D139" s="5">
-        <v>97064415</v>
+        <v>97036910</v>
       </c>
       <c r="E139" s="5">
-        <v>97081118</v>
+        <v>97064068</v>
       </c>
       <c r="F139" s="11"/>
       <c r="G139" s="11"/>
@@ -5287,19 +5283,19 @@
     </row>
     <row r="140" spans="1:22" ht="14.4">
       <c r="A140" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="B140" s="21"/>
-      <c r="C140" s="21"/>
+        <v>146</v>
+      </c>
+      <c r="B140" s="16"/>
+      <c r="C140" s="14"/>
       <c r="D140" s="5">
-        <v>97084201</v>
+        <v>97064415</v>
       </c>
       <c r="E140" s="5">
-        <v>97084290</v>
-      </c>
-      <c r="F140" s="4"/>
-      <c r="G140" s="4"/>
-      <c r="H140" s="4"/>
+        <v>97081118</v>
+      </c>
+      <c r="F140" s="11"/>
+      <c r="G140" s="11"/>
+      <c r="H140" s="11"/>
       <c r="I140" s="2"/>
       <c r="J140" s="2"/>
       <c r="K140" s="2"/>
@@ -5317,19 +5313,19 @@
     </row>
     <row r="141" spans="1:22" ht="14.4">
       <c r="A141" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="B141" s="16"/>
-      <c r="C141" s="14"/>
+        <v>147</v>
+      </c>
+      <c r="B141" s="21"/>
+      <c r="C141" s="21"/>
       <c r="D141" s="5">
-        <v>97086225</v>
+        <v>97084201</v>
       </c>
       <c r="E141" s="5">
-        <v>97105001</v>
-      </c>
-      <c r="F141" s="11"/>
-      <c r="G141" s="11"/>
-      <c r="H141" s="11"/>
+        <v>97084290</v>
+      </c>
+      <c r="F141" s="4"/>
+      <c r="G141" s="4"/>
+      <c r="H141" s="4"/>
       <c r="I141" s="2"/>
       <c r="J141" s="2"/>
       <c r="K141" s="2"/>
@@ -5347,15 +5343,15 @@
     </row>
     <row r="142" spans="1:22" ht="14.4">
       <c r="A142" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B142" s="16"/>
-      <c r="C142" s="20"/>
+      <c r="C142" s="14"/>
       <c r="D142" s="5">
-        <v>97109423</v>
+        <v>97086225</v>
       </c>
       <c r="E142" s="5">
-        <v>97126962</v>
+        <v>97105001</v>
       </c>
       <c r="F142" s="11"/>
       <c r="G142" s="11"/>
@@ -5377,15 +5373,15 @@
     </row>
     <row r="143" spans="1:22" ht="14.4">
       <c r="A143" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B143" s="16"/>
       <c r="C143" s="20"/>
       <c r="D143" s="5">
-        <v>97126904</v>
+        <v>97109423</v>
       </c>
       <c r="E143" s="5">
-        <v>97135588</v>
+        <v>97126962</v>
       </c>
       <c r="F143" s="11"/>
       <c r="G143" s="11"/>
@@ -5407,19 +5403,19 @@
     </row>
     <row r="144" spans="1:22" ht="14.4">
       <c r="A144" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="B144" s="21"/>
-      <c r="C144" s="21"/>
+        <v>150</v>
+      </c>
+      <c r="B144" s="16"/>
+      <c r="C144" s="20"/>
       <c r="D144" s="5">
-        <v>97128891</v>
+        <v>97126904</v>
       </c>
       <c r="E144" s="5">
-        <v>97128963</v>
-      </c>
-      <c r="F144" s="4"/>
-      <c r="G144" s="4"/>
-      <c r="H144" s="4"/>
+        <v>97135588</v>
+      </c>
+      <c r="F144" s="11"/>
+      <c r="G144" s="11"/>
+      <c r="H144" s="11"/>
       <c r="I144" s="2"/>
       <c r="J144" s="2"/>
       <c r="K144" s="2"/>
@@ -5437,15 +5433,15 @@
     </row>
     <row r="145" spans="1:22" ht="14.4">
       <c r="A145" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="B145" s="11"/>
-      <c r="C145" s="22"/>
+        <v>151</v>
+      </c>
+      <c r="B145" s="21"/>
+      <c r="C145" s="21"/>
       <c r="D145" s="5">
-        <v>97218753</v>
+        <v>97128891</v>
       </c>
       <c r="E145" s="5">
-        <v>97222647</v>
+        <v>97128963</v>
       </c>
       <c r="F145" s="4"/>
       <c r="G145" s="4"/>
@@ -5467,15 +5463,15 @@
     </row>
     <row r="146" spans="1:22" ht="14.4">
       <c r="A146" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B146" s="11"/>
-      <c r="C146" s="20"/>
+      <c r="C146" s="22"/>
       <c r="D146" s="5">
-        <v>108869996</v>
+        <v>97218753</v>
       </c>
       <c r="E146" s="5">
-        <v>108870162</v>
+        <v>97222647</v>
       </c>
       <c r="F146" s="4"/>
       <c r="G146" s="4"/>
@@ -5497,19 +5493,19 @@
     </row>
     <row r="147" spans="1:22" ht="14.4">
       <c r="A147" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="B147" s="16"/>
-      <c r="C147" s="1"/>
+        <v>153</v>
+      </c>
+      <c r="B147" s="11"/>
+      <c r="C147" s="20"/>
       <c r="D147" s="5">
-        <v>108977758</v>
+        <v>108869996</v>
       </c>
       <c r="E147" s="5">
-        <v>108987010</v>
-      </c>
-      <c r="F147" s="11"/>
-      <c r="G147" s="11"/>
-      <c r="H147" s="11"/>
+        <v>108870162</v>
+      </c>
+      <c r="F147" s="4"/>
+      <c r="G147" s="4"/>
+      <c r="H147" s="4"/>
       <c r="I147" s="2"/>
       <c r="J147" s="2"/>
       <c r="K147" s="2"/>
@@ -5527,15 +5523,15 @@
     </row>
     <row r="148" spans="1:22" ht="14.4">
       <c r="A148" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B148" s="16"/>
       <c r="C148" s="1"/>
       <c r="D148" s="5">
-        <v>109624582</v>
+        <v>108977758</v>
       </c>
       <c r="E148" s="5">
-        <v>109891384</v>
+        <v>108987010</v>
       </c>
       <c r="F148" s="11"/>
       <c r="G148" s="11"/>
@@ -5557,19 +5553,19 @@
     </row>
     <row r="149" spans="1:22" ht="14.4">
       <c r="A149" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="B149" s="4"/>
-      <c r="C149" s="12"/>
+        <v>155</v>
+      </c>
+      <c r="B149" s="16"/>
+      <c r="C149" s="1"/>
       <c r="D149" s="5">
-        <v>109654627</v>
+        <v>109624582</v>
       </c>
       <c r="E149" s="5">
-        <v>109656668</v>
-      </c>
-      <c r="F149" s="4"/>
-      <c r="G149" s="4"/>
-      <c r="H149" s="4"/>
+        <v>109891384</v>
+      </c>
+      <c r="F149" s="11"/>
+      <c r="G149" s="11"/>
+      <c r="H149" s="11"/>
       <c r="I149" s="2"/>
       <c r="J149" s="2"/>
       <c r="K149" s="2"/>
@@ -5587,15 +5583,15 @@
     </row>
     <row r="150" spans="1:22" ht="14.4">
       <c r="A150" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B150" s="4"/>
-      <c r="C150" s="3"/>
+      <c r="C150" s="12"/>
       <c r="D150" s="5">
-        <v>109705012</v>
+        <v>109654627</v>
       </c>
       <c r="E150" s="5">
-        <v>109711074</v>
+        <v>109656668</v>
       </c>
       <c r="F150" s="4"/>
       <c r="G150" s="4"/>
@@ -5617,15 +5613,15 @@
     </row>
     <row r="151" spans="1:22" ht="14.4">
       <c r="A151" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B151" s="4"/>
-      <c r="C151" s="12"/>
+      <c r="C151" s="3"/>
       <c r="D151" s="5">
-        <v>110006450</v>
+        <v>109705012</v>
       </c>
       <c r="E151" s="5">
-        <v>110008114</v>
+        <v>109711074</v>
       </c>
       <c r="F151" s="4"/>
       <c r="G151" s="4"/>
@@ -5647,15 +5643,15 @@
     </row>
     <row r="152" spans="1:22" ht="14.4">
       <c r="A152" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B152" s="4"/>
       <c r="C152" s="12"/>
       <c r="D152" s="5">
-        <v>110007825</v>
+        <v>110006450</v>
       </c>
       <c r="E152" s="5">
-        <v>110021805</v>
+        <v>110008114</v>
       </c>
       <c r="F152" s="4"/>
       <c r="G152" s="4"/>
@@ -5677,15 +5673,15 @@
     </row>
     <row r="153" spans="1:22" ht="14.4">
       <c r="A153" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B153" s="4"/>
       <c r="C153" s="12"/>
       <c r="D153" s="5">
-        <v>110105303</v>
+        <v>110007825</v>
       </c>
       <c r="E153" s="5">
-        <v>110109142</v>
+        <v>110021805</v>
       </c>
       <c r="F153" s="4"/>
       <c r="G153" s="4"/>
@@ -5707,15 +5703,15 @@
     </row>
     <row r="154" spans="1:22" ht="14.4">
       <c r="A154" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B154" s="4"/>
       <c r="C154" s="12"/>
       <c r="D154" s="5">
-        <v>110131156</v>
+        <v>110105303</v>
       </c>
       <c r="E154" s="5">
-        <v>110330653</v>
+        <v>110109142</v>
       </c>
       <c r="F154" s="4"/>
       <c r="G154" s="4"/>
@@ -5737,15 +5733,15 @@
     </row>
     <row r="155" spans="1:22" ht="14.4">
       <c r="A155" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B155" s="4"/>
       <c r="C155" s="12"/>
       <c r="D155" s="5">
-        <v>110482876</v>
+        <v>110131156</v>
       </c>
       <c r="E155" s="5">
-        <v>110512320</v>
+        <v>110330653</v>
       </c>
       <c r="F155" s="4"/>
       <c r="G155" s="4"/>
@@ -5767,15 +5763,15 @@
     </row>
     <row r="156" spans="1:22" ht="14.4">
       <c r="A156" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B156" s="4"/>
       <c r="C156" s="12"/>
       <c r="D156" s="5">
-        <v>110605285</v>
+        <v>110482876</v>
       </c>
       <c r="E156" s="5">
-        <v>110611613</v>
+        <v>110512320</v>
       </c>
       <c r="F156" s="4"/>
       <c r="G156" s="4"/>
@@ -5797,15 +5793,15 @@
     </row>
     <row r="157" spans="1:22" ht="14.4">
       <c r="A157" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B157" s="4"/>
       <c r="C157" s="12"/>
       <c r="D157" s="5">
-        <v>110641897</v>
+        <v>110605285</v>
       </c>
       <c r="E157" s="5">
-        <v>110653517</v>
+        <v>110611613</v>
       </c>
       <c r="F157" s="4"/>
       <c r="G157" s="4"/>
@@ -5827,15 +5823,15 @@
     </row>
     <row r="158" spans="1:22" ht="14.4">
       <c r="A158" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="B158" s="6"/>
-      <c r="C158" s="7"/>
-      <c r="D158" s="23">
-        <v>113460909</v>
-      </c>
-      <c r="E158" s="23">
-        <v>113465343</v>
+        <v>164</v>
+      </c>
+      <c r="B158" s="4"/>
+      <c r="C158" s="12"/>
+      <c r="D158" s="5">
+        <v>110641897</v>
+      </c>
+      <c r="E158" s="5">
+        <v>110653517</v>
       </c>
       <c r="F158" s="4"/>
       <c r="G158" s="4"/>
@@ -5857,15 +5853,15 @@
     </row>
     <row r="159" spans="1:22" ht="14.4">
       <c r="A159" s="27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B159" s="6"/>
       <c r="C159" s="7"/>
       <c r="D159" s="23">
-        <v>114039627</v>
+        <v>113460909</v>
       </c>
       <c r="E159" s="23">
-        <v>114044419</v>
+        <v>113465343</v>
       </c>
       <c r="F159" s="4"/>
       <c r="G159" s="4"/>
@@ -5887,15 +5883,15 @@
     </row>
     <row r="160" spans="1:22" ht="14.4">
       <c r="A160" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B160" s="6"/>
       <c r="C160" s="7"/>
       <c r="D160" s="23">
-        <v>114205077</v>
+        <v>114039627</v>
       </c>
       <c r="E160" s="23">
-        <v>114214900</v>
+        <v>114044419</v>
       </c>
       <c r="F160" s="4"/>
       <c r="G160" s="4"/>
@@ -5917,15 +5913,15 @@
     </row>
     <row r="161" spans="1:22" ht="14.4">
       <c r="A161" s="27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B161" s="6"/>
       <c r="C161" s="7"/>
       <c r="D161" s="23">
-        <v>114567590</v>
+        <v>114205077</v>
       </c>
       <c r="E161" s="23">
-        <v>114574104</v>
+        <v>114214900</v>
       </c>
       <c r="F161" s="4"/>
       <c r="G161" s="4"/>
@@ -5947,15 +5943,15 @@
     </row>
     <row r="162" spans="1:22" ht="14.4">
       <c r="A162" s="27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B162" s="6"/>
       <c r="C162" s="7"/>
       <c r="D162" s="23">
-        <v>114638336</v>
+        <v>114567590</v>
       </c>
       <c r="E162" s="23">
-        <v>114643543</v>
+        <v>114574104</v>
       </c>
       <c r="F162" s="4"/>
       <c r="G162" s="4"/>
@@ -5977,15 +5973,15 @@
     </row>
     <row r="163" spans="1:22" ht="14.4">
       <c r="A163" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B163" s="6"/>
       <c r="C163" s="7"/>
       <c r="D163" s="23">
-        <v>114974326</v>
+        <v>114638336</v>
       </c>
       <c r="E163" s="23">
-        <v>115192808</v>
+        <v>114643543</v>
       </c>
       <c r="F163" s="4"/>
       <c r="G163" s="4"/>
@@ -6007,15 +6003,15 @@
     </row>
     <row r="164" spans="1:22" ht="14.4">
       <c r="A164" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B164" s="6"/>
       <c r="C164" s="7"/>
       <c r="D164" s="23">
-        <v>115334226</v>
+        <v>114974326</v>
       </c>
       <c r="E164" s="23">
-        <v>115335879</v>
+        <v>115192808</v>
       </c>
       <c r="F164" s="4"/>
       <c r="G164" s="4"/>
@@ -6037,15 +6033,15 @@
     </row>
     <row r="165" spans="1:22" ht="14.4">
       <c r="A165" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B165" s="6"/>
       <c r="C165" s="7"/>
       <c r="D165" s="23">
-        <v>115626920</v>
+        <v>115334226</v>
       </c>
       <c r="E165" s="23">
-        <v>115636639</v>
+        <v>115335879</v>
       </c>
       <c r="F165" s="4"/>
       <c r="G165" s="4"/>
@@ -6067,15 +6063,15 @@
     </row>
     <row r="166" spans="1:22" ht="14.4">
       <c r="A166" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B166" s="6"/>
       <c r="C166" s="7"/>
       <c r="D166" s="23">
-        <v>115725079</v>
+        <v>115626920</v>
       </c>
       <c r="E166" s="23">
-        <v>115746451</v>
+        <v>115636639</v>
       </c>
       <c r="F166" s="4"/>
       <c r="G166" s="4"/>
@@ -6097,15 +6093,15 @@
     </row>
     <row r="167" spans="1:22" ht="14.4">
       <c r="A167" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B167" s="6"/>
       <c r="C167" s="7"/>
       <c r="D167" s="23">
-        <v>115759698</v>
+        <v>115725079</v>
       </c>
       <c r="E167" s="23">
-        <v>115774070</v>
+        <v>115746451</v>
       </c>
       <c r="F167" s="4"/>
       <c r="G167" s="4"/>
@@ -6127,15 +6123,15 @@
     </row>
     <row r="168" spans="1:22" ht="14.4">
       <c r="A168" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B168" s="6"/>
       <c r="C168" s="7"/>
       <c r="D168" s="23">
-        <v>115761181</v>
+        <v>115759698</v>
       </c>
       <c r="E168" s="23">
-        <v>115761777</v>
+        <v>115774070</v>
       </c>
       <c r="F168" s="4"/>
       <c r="G168" s="4"/>
@@ -6157,15 +6153,15 @@
     </row>
     <row r="169" spans="1:22" ht="14.4">
       <c r="A169" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B169" s="6"/>
       <c r="C169" s="7"/>
       <c r="D169" s="23">
-        <v>115795806</v>
+        <v>115761181</v>
       </c>
       <c r="E169" s="23">
-        <v>115830521</v>
+        <v>115761777</v>
       </c>
       <c r="F169" s="4"/>
       <c r="G169" s="4"/>
@@ -6187,15 +6183,15 @@
     </row>
     <row r="170" spans="1:22" ht="14.4">
       <c r="A170" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B170" s="6"/>
       <c r="C170" s="7"/>
       <c r="D170" s="23">
-        <v>115895606</v>
+        <v>115795806</v>
       </c>
       <c r="E170" s="23">
-        <v>115924433</v>
+        <v>115830521</v>
       </c>
       <c r="F170" s="4"/>
       <c r="G170" s="4"/>
@@ -6217,15 +6213,15 @@
     </row>
     <row r="171" spans="1:22" ht="14.4">
       <c r="A171" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B171" s="6"/>
       <c r="C171" s="7"/>
       <c r="D171" s="23">
-        <v>115940485</v>
+        <v>115895606</v>
       </c>
       <c r="E171" s="23">
-        <v>115948547</v>
+        <v>115924433</v>
       </c>
       <c r="F171" s="4"/>
       <c r="G171" s="4"/>
@@ -6247,15 +6243,15 @@
     </row>
     <row r="172" spans="1:22" ht="14.4">
       <c r="A172" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B172" s="6"/>
       <c r="C172" s="7"/>
       <c r="D172" s="23">
-        <v>115952522</v>
+        <v>115940485</v>
       </c>
       <c r="E172" s="23">
-        <v>115953478</v>
+        <v>115948547</v>
       </c>
       <c r="F172" s="4"/>
       <c r="G172" s="4"/>
@@ -6277,15 +6273,15 @@
     </row>
     <row r="173" spans="1:22" ht="14.4">
       <c r="A173" s="27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B173" s="6"/>
       <c r="C173" s="7"/>
       <c r="D173" s="23">
-        <v>116180918</v>
+        <v>115952522</v>
       </c>
       <c r="E173" s="23">
-        <v>116185772</v>
+        <v>115953478</v>
       </c>
       <c r="F173" s="4"/>
       <c r="G173" s="4"/>
@@ -6307,15 +6303,15 @@
     </row>
     <row r="174" spans="1:22" ht="14.4">
       <c r="A174" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="B174" s="4"/>
-      <c r="C174" s="12"/>
-      <c r="D174" s="5">
-        <v>142144336</v>
-      </c>
-      <c r="E174" s="5">
-        <v>142147673</v>
+        <v>180</v>
+      </c>
+      <c r="B174" s="6"/>
+      <c r="C174" s="7"/>
+      <c r="D174" s="23">
+        <v>116180918</v>
+      </c>
+      <c r="E174" s="23">
+        <v>116185772</v>
       </c>
       <c r="F174" s="4"/>
       <c r="G174" s="4"/>
@@ -6337,15 +6333,15 @@
     </row>
     <row r="175" spans="1:22" ht="14.4">
       <c r="A175" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B175" s="4"/>
       <c r="C175" s="12"/>
       <c r="D175" s="5">
-        <v>142195365</v>
+        <v>142144336</v>
       </c>
       <c r="E175" s="5">
-        <v>142198459</v>
+        <v>142147673</v>
       </c>
       <c r="F175" s="4"/>
       <c r="G175" s="4"/>
@@ -6367,15 +6363,15 @@
     </row>
     <row r="176" spans="1:22" ht="14.4">
       <c r="A176" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B176" s="4"/>
       <c r="C176" s="12"/>
       <c r="D176" s="5">
-        <v>142210652</v>
+        <v>142195365</v>
       </c>
       <c r="E176" s="5">
-        <v>142215120</v>
+        <v>142198459</v>
       </c>
       <c r="F176" s="4"/>
       <c r="G176" s="4"/>
@@ -6397,15 +6393,15 @@
     </row>
     <row r="177" spans="1:22" ht="14.4">
       <c r="A177" s="27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B177" s="4"/>
       <c r="C177" s="12"/>
       <c r="D177" s="5">
-        <v>142244254</v>
+        <v>142210652</v>
       </c>
       <c r="E177" s="5">
-        <v>142266328</v>
+        <v>142215120</v>
       </c>
       <c r="F177" s="4"/>
       <c r="G177" s="4"/>
@@ -6427,15 +6423,15 @@
     </row>
     <row r="178" spans="1:22" ht="14.4">
       <c r="A178" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B178" s="4"/>
       <c r="C178" s="12"/>
       <c r="D178" s="5">
-        <v>142279670</v>
+        <v>142244254</v>
       </c>
       <c r="E178" s="5">
-        <v>142319559</v>
+        <v>142266328</v>
       </c>
       <c r="F178" s="4"/>
       <c r="G178" s="4"/>
@@ -6457,15 +6453,15 @@
     </row>
     <row r="179" spans="1:22" ht="14.4">
       <c r="A179" s="27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B179" s="4"/>
       <c r="C179" s="12"/>
       <c r="D179" s="5">
-        <v>142343036</v>
+        <v>142279670</v>
       </c>
       <c r="E179" s="5">
-        <v>142357475</v>
+        <v>142319559</v>
       </c>
       <c r="F179" s="4"/>
       <c r="G179" s="4"/>
@@ -6487,15 +6483,15 @@
     </row>
     <row r="180" spans="1:22" ht="14.4">
       <c r="A180" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B180" s="4"/>
       <c r="C180" s="12"/>
       <c r="D180" s="5">
-        <v>142382950</v>
+        <v>142343036</v>
       </c>
       <c r="E180" s="5">
-        <v>142456016</v>
+        <v>142357475</v>
       </c>
       <c r="F180" s="4"/>
       <c r="G180" s="4"/>
@@ -6517,15 +6513,15 @@
     </row>
     <row r="181" spans="1:22" ht="14.4">
       <c r="A181" s="27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B181" s="4"/>
-      <c r="C181" s="13"/>
+      <c r="C181" s="12"/>
       <c r="D181" s="5">
-        <v>142514732</v>
+        <v>142382950</v>
       </c>
       <c r="E181" s="5">
-        <v>142621037</v>
+        <v>142456016</v>
       </c>
       <c r="F181" s="4"/>
       <c r="G181" s="4"/>
@@ -6547,15 +6543,15 @@
     </row>
     <row r="182" spans="1:22" ht="14.4">
       <c r="A182" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B182" s="4"/>
-      <c r="C182" s="12"/>
+      <c r="C182" s="13"/>
       <c r="D182" s="5">
-        <v>142670674</v>
+        <v>142514732</v>
       </c>
       <c r="E182" s="5">
-        <v>142689333</v>
+        <v>142621037</v>
       </c>
       <c r="F182" s="4"/>
       <c r="G182" s="4"/>
@@ -6577,15 +6573,15 @@
     </row>
     <row r="183" spans="1:22" ht="14.4">
       <c r="A183" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B183" s="4"/>
       <c r="C183" s="12"/>
       <c r="D183" s="5">
-        <v>142705607</v>
+        <v>142670674</v>
       </c>
       <c r="E183" s="5">
-        <v>142717197</v>
+        <v>142689333</v>
       </c>
       <c r="F183" s="4"/>
       <c r="G183" s="4"/>
@@ -6607,15 +6603,15 @@
     </row>
     <row r="184" spans="1:22" ht="14.4">
       <c r="A184" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B184" s="4"/>
       <c r="C184" s="12"/>
       <c r="D184" s="5">
-        <v>142744432</v>
+        <v>142705607</v>
       </c>
       <c r="E184" s="5">
-        <v>142789033</v>
+        <v>142717197</v>
       </c>
       <c r="F184" s="4"/>
       <c r="G184" s="4"/>
@@ -6637,15 +6633,15 @@
     </row>
     <row r="185" spans="1:22" ht="14.4">
       <c r="A185" s="27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B185" s="4"/>
       <c r="C185" s="12"/>
       <c r="D185" s="5">
-        <v>144900016</v>
+        <v>142744432</v>
       </c>
       <c r="E185" s="5">
-        <v>144991569</v>
+        <v>142789033</v>
       </c>
       <c r="F185" s="4"/>
       <c r="G185" s="4"/>
@@ -6667,15 +6663,15 @@
     </row>
     <row r="186" spans="1:22" ht="14.4">
       <c r="A186" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B186" s="4"/>
       <c r="C186" s="12"/>
       <c r="D186" s="5">
-        <v>145035446</v>
+        <v>144900016</v>
       </c>
       <c r="E186" s="5">
-        <v>145048712</v>
+        <v>144991569</v>
       </c>
       <c r="F186" s="4"/>
       <c r="G186" s="4"/>
@@ -6697,15 +6693,15 @@
     </row>
     <row r="187" spans="1:22" ht="14.4">
       <c r="A187" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B187" s="4"/>
       <c r="C187" s="12"/>
       <c r="D187" s="5">
-        <v>145152446</v>
+        <v>145035446</v>
       </c>
       <c r="E187" s="5">
-        <v>145246309</v>
+        <v>145048712</v>
       </c>
       <c r="F187" s="4"/>
       <c r="G187" s="4"/>
@@ -6727,15 +6723,15 @@
     </row>
     <row r="188" spans="1:22" ht="14.4">
       <c r="A188" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B188" s="4"/>
       <c r="C188" s="12"/>
       <c r="D188" s="5">
-        <v>145249313</v>
+        <v>145152446</v>
       </c>
       <c r="E188" s="5">
-        <v>145275187</v>
+        <v>145246309</v>
       </c>
       <c r="F188" s="4"/>
       <c r="G188" s="4"/>
@@ -6757,15 +6753,15 @@
     </row>
     <row r="189" spans="1:22" ht="14.4">
       <c r="A189" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B189" s="4"/>
       <c r="C189" s="12"/>
       <c r="D189" s="5">
-        <v>145344482</v>
+        <v>145249313</v>
       </c>
       <c r="E189" s="5">
-        <v>145581973</v>
+        <v>145275187</v>
       </c>
       <c r="F189" s="4"/>
       <c r="G189" s="4"/>
@@ -6787,15 +6783,15 @@
     </row>
     <row r="190" spans="1:22" ht="14.4">
       <c r="A190" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B190" s="4"/>
       <c r="C190" s="12"/>
       <c r="D190" s="5">
-        <v>145590006</v>
+        <v>145344482</v>
       </c>
       <c r="E190" s="5">
-        <v>145591118</v>
+        <v>145581973</v>
       </c>
       <c r="F190" s="4"/>
       <c r="G190" s="4"/>
@@ -6817,15 +6813,15 @@
     </row>
     <row r="191" spans="1:22" ht="14.4">
       <c r="A191" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B191" s="4"/>
       <c r="C191" s="12"/>
       <c r="D191" s="5">
-        <v>145631195</v>
+        <v>145590006</v>
       </c>
       <c r="E191" s="5">
-        <v>145652325</v>
+        <v>145591118</v>
       </c>
       <c r="F191" s="4"/>
       <c r="G191" s="4"/>
@@ -6847,15 +6843,15 @@
     </row>
     <row r="192" spans="1:22" ht="14.4">
       <c r="A192" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B192" s="4"/>
       <c r="C192" s="12"/>
       <c r="D192" s="5">
-        <v>145768042</v>
+        <v>145631195</v>
       </c>
       <c r="E192" s="5">
-        <v>145799845</v>
+        <v>145652325</v>
       </c>
       <c r="F192" s="4"/>
       <c r="G192" s="4"/>
@@ -6877,15 +6873,15 @@
     </row>
     <row r="193" spans="1:22" ht="14.4">
       <c r="A193" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B193" s="4"/>
       <c r="C193" s="12"/>
       <c r="D193" s="5">
-        <v>145809671</v>
+        <v>145768042</v>
       </c>
       <c r="E193" s="5">
-        <v>145824726</v>
+        <v>145799845</v>
       </c>
       <c r="F193" s="4"/>
       <c r="G193" s="4"/>
@@ -6907,15 +6903,15 @@
     </row>
     <row r="194" spans="1:22" ht="14.4">
       <c r="A194" s="27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B194" s="4"/>
       <c r="C194" s="12"/>
       <c r="D194" s="5">
-        <v>145826815</v>
+        <v>145809671</v>
       </c>
       <c r="E194" s="5">
-        <v>145847568</v>
+        <v>145824726</v>
       </c>
       <c r="F194" s="4"/>
       <c r="G194" s="4"/>
@@ -6937,15 +6933,15 @@
     </row>
     <row r="195" spans="1:22" ht="14.4">
       <c r="A195" s="27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B195" s="4"/>
       <c r="C195" s="12"/>
       <c r="D195" s="5">
-        <v>145851416</v>
+        <v>145826815</v>
       </c>
       <c r="E195" s="5">
-        <v>145883591</v>
+        <v>145847568</v>
       </c>
       <c r="F195" s="4"/>
       <c r="G195" s="4"/>
@@ -6967,15 +6963,15 @@
     </row>
     <row r="196" spans="1:22" ht="14.4">
       <c r="A196" s="27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B196" s="4"/>
       <c r="C196" s="12"/>
       <c r="D196" s="5">
-        <v>145893289</v>
+        <v>145851416</v>
       </c>
       <c r="E196" s="5">
-        <v>145937594</v>
+        <v>145883591</v>
       </c>
       <c r="F196" s="4"/>
       <c r="G196" s="4"/>
@@ -6997,15 +6993,15 @@
     </row>
     <row r="197" spans="1:22" ht="14.4">
       <c r="A197" s="27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B197" s="4"/>
       <c r="C197" s="12"/>
       <c r="D197" s="5">
-        <v>145937640</v>
+        <v>145893289</v>
       </c>
       <c r="E197" s="5">
-        <v>145945394</v>
+        <v>145937594</v>
       </c>
       <c r="F197" s="4"/>
       <c r="G197" s="4"/>
@@ -7027,15 +7023,15 @@
     </row>
     <row r="198" spans="1:22" ht="14.4">
       <c r="A198" s="27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B198" s="4"/>
       <c r="C198" s="12"/>
       <c r="D198" s="5">
-        <v>145947155</v>
+        <v>145937640</v>
       </c>
       <c r="E198" s="5">
-        <v>145959034</v>
+        <v>145945394</v>
       </c>
       <c r="F198" s="4"/>
       <c r="G198" s="4"/>
@@ -7057,15 +7053,15 @@
     </row>
     <row r="199" spans="1:22" ht="14.4">
       <c r="A199" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B199" s="4"/>
       <c r="C199" s="12"/>
       <c r="D199" s="5">
-        <v>145965792</v>
+        <v>145947155</v>
       </c>
       <c r="E199" s="5">
-        <v>146072360</v>
+        <v>145959034</v>
       </c>
       <c r="F199" s="4"/>
       <c r="G199" s="4"/>
@@ -7087,15 +7083,15 @@
     </row>
     <row r="200" spans="1:22" ht="14.4">
       <c r="A200" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B200" s="4"/>
       <c r="C200" s="12"/>
       <c r="D200" s="5">
-        <v>146074561</v>
+        <v>145965792</v>
       </c>
       <c r="E200" s="5">
-        <v>146085374</v>
+        <v>146072360</v>
       </c>
       <c r="F200" s="4"/>
       <c r="G200" s="4"/>
@@ -7117,15 +7113,15 @@
     </row>
     <row r="201" spans="1:22" ht="14.4">
       <c r="A201" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B201" s="4"/>
       <c r="C201" s="12"/>
       <c r="D201" s="5">
-        <v>146077830</v>
+        <v>146074561</v>
       </c>
       <c r="E201" s="5">
-        <v>146078115</v>
+        <v>146085374</v>
       </c>
       <c r="F201" s="4"/>
       <c r="G201" s="4"/>
@@ -7147,15 +7143,15 @@
     </row>
     <row r="202" spans="1:22" ht="14.4">
       <c r="A202" s="27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B202" s="4"/>
       <c r="C202" s="12"/>
       <c r="D202" s="5">
-        <v>146085595</v>
+        <v>146077830</v>
       </c>
       <c r="E202" s="5">
-        <v>146195343</v>
+        <v>146078115</v>
       </c>
       <c r="F202" s="4"/>
       <c r="G202" s="4"/>
@@ -7177,15 +7173,15 @@
     </row>
     <row r="203" spans="1:22" ht="14.4">
       <c r="A203" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B203" s="4"/>
       <c r="C203" s="12"/>
       <c r="D203" s="5">
-        <v>146236243</v>
+        <v>146085595</v>
       </c>
       <c r="E203" s="5">
-        <v>146243445</v>
+        <v>146195343</v>
       </c>
       <c r="F203" s="4"/>
       <c r="G203" s="4"/>
@@ -7207,15 +7203,15 @@
     </row>
     <row r="204" spans="1:22" ht="14.4">
       <c r="A204" s="27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B204" s="4"/>
       <c r="C204" s="12"/>
       <c r="D204" s="5">
-        <v>146282780</v>
+        <v>146236243</v>
       </c>
       <c r="E204" s="5">
-        <v>146307587</v>
+        <v>146243445</v>
       </c>
       <c r="F204" s="4"/>
       <c r="G204" s="4"/>
@@ -7237,15 +7233,15 @@
     </row>
     <row r="205" spans="1:22" ht="14.4">
       <c r="A205" s="27" t="s">
-        <v>212</v>
-      </c>
-      <c r="B205" s="11"/>
-      <c r="C205" s="20"/>
+        <v>211</v>
+      </c>
+      <c r="B205" s="4"/>
+      <c r="C205" s="12"/>
       <c r="D205" s="5">
-        <v>146452171</v>
+        <v>146282780</v>
       </c>
       <c r="E205" s="5">
-        <v>146480596</v>
+        <v>146307587</v>
       </c>
       <c r="F205" s="4"/>
       <c r="G205" s="4"/>
@@ -7267,19 +7263,19 @@
     </row>
     <row r="206" spans="1:22" ht="14.4">
       <c r="A206" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B206" s="11"/>
       <c r="C206" s="20"/>
       <c r="D206" s="5">
-        <v>146484584</v>
+        <v>146452171</v>
       </c>
       <c r="E206" s="5">
-        <v>146528594</v>
-      </c>
-      <c r="F206" s="11"/>
-      <c r="G206" s="11"/>
-      <c r="H206" s="11"/>
+        <v>146480596</v>
+      </c>
+      <c r="F206" s="4"/>
+      <c r="G206" s="4"/>
+      <c r="H206" s="4"/>
       <c r="I206" s="2"/>
       <c r="J206" s="2"/>
       <c r="K206" s="2"/>
@@ -7297,15 +7293,15 @@
     </row>
     <row r="207" spans="1:22" ht="14.4">
       <c r="A207" s="27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B207" s="11"/>
-      <c r="C207" s="24"/>
+      <c r="C207" s="20"/>
       <c r="D207" s="5">
-        <v>146768806</v>
+        <v>146484584</v>
       </c>
       <c r="E207" s="5">
-        <v>146779619</v>
+        <v>146528594</v>
       </c>
       <c r="F207" s="11"/>
       <c r="G207" s="11"/>
@@ -7327,15 +7323,15 @@
     </row>
     <row r="208" spans="1:22" ht="14.4">
       <c r="A208" s="27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B208" s="11"/>
-      <c r="C208" s="25"/>
+      <c r="C208" s="24"/>
       <c r="D208" s="5">
-        <v>153477636</v>
+        <v>146768806</v>
       </c>
       <c r="E208" s="5">
-        <v>153498961</v>
+        <v>146779619</v>
       </c>
       <c r="F208" s="11"/>
       <c r="G208" s="11"/>
@@ -7357,15 +7353,15 @@
     </row>
     <row r="209" spans="1:22" ht="14.4">
       <c r="A209" s="27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B209" s="11"/>
-      <c r="C209" s="13"/>
+      <c r="C209" s="25"/>
       <c r="D209" s="5">
-        <v>153722829</v>
+        <v>153477636</v>
       </c>
       <c r="E209" s="5">
-        <v>153936148</v>
+        <v>153498961</v>
       </c>
       <c r="F209" s="11"/>
       <c r="G209" s="11"/>
@@ -7387,15 +7383,15 @@
     </row>
     <row r="210" spans="1:22" ht="14.4">
       <c r="A210" s="27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B210" s="11"/>
       <c r="C210" s="13"/>
       <c r="D210" s="5">
-        <v>153936559</v>
+        <v>153722829</v>
       </c>
       <c r="E210" s="5">
-        <v>154524620</v>
+        <v>153936148</v>
       </c>
       <c r="F210" s="11"/>
       <c r="G210" s="11"/>
@@ -7417,19 +7413,19 @@
     </row>
     <row r="211" spans="1:22" ht="14.4">
       <c r="A211" s="27" t="s">
-        <v>218</v>
-      </c>
-      <c r="B211" s="4"/>
-      <c r="C211" s="12"/>
+        <v>217</v>
+      </c>
+      <c r="B211" s="11"/>
+      <c r="C211" s="13"/>
       <c r="D211" s="5">
-        <v>154244176</v>
+        <v>153936559</v>
       </c>
       <c r="E211" s="5">
-        <v>154244247</v>
-      </c>
-      <c r="F211" s="4"/>
-      <c r="G211" s="4"/>
-      <c r="H211" s="4"/>
+        <v>154524620</v>
+      </c>
+      <c r="F211" s="11"/>
+      <c r="G211" s="11"/>
+      <c r="H211" s="11"/>
       <c r="I211" s="2"/>
       <c r="J211" s="2"/>
       <c r="K211" s="2"/>
@@ -7447,19 +7443,19 @@
     </row>
     <row r="212" spans="1:22" ht="14.4">
       <c r="A212" s="27" t="s">
-        <v>219</v>
-      </c>
-      <c r="B212" s="11"/>
-      <c r="C212" s="13"/>
+        <v>218</v>
+      </c>
+      <c r="B212" s="4"/>
+      <c r="C212" s="12"/>
       <c r="D212" s="5">
-        <v>155262593</v>
+        <v>154244176</v>
       </c>
       <c r="E212" s="5">
-        <v>155364610</v>
-      </c>
-      <c r="F212" s="11"/>
-      <c r="G212" s="11"/>
-      <c r="H212" s="11"/>
+        <v>154244247</v>
+      </c>
+      <c r="F212" s="4"/>
+      <c r="G212" s="4"/>
+      <c r="H212" s="4"/>
       <c r="I212" s="2"/>
       <c r="J212" s="2"/>
       <c r="K212" s="2"/>
@@ -7477,15 +7473,15 @@
     </row>
     <row r="213" spans="1:22" ht="14.4">
       <c r="A213" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B213" s="11"/>
       <c r="C213" s="13"/>
       <c r="D213" s="5">
-        <v>156184812</v>
+        <v>155262593</v>
       </c>
       <c r="E213" s="5">
-        <v>156650711</v>
+        <v>155364610</v>
       </c>
       <c r="F213" s="11"/>
       <c r="G213" s="11"/>
@@ -7505,31 +7501,35 @@
       <c r="U213" s="2"/>
       <c r="V213" s="2"/>
     </row>
-    <row r="214" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A214" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B214" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C214" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D214" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E214" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F214" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="G214" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="H214" s="26" t="s">
-        <v>9</v>
-      </c>
+    <row r="214" spans="1:22" ht="14.4">
+      <c r="A214" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="B214" s="11"/>
+      <c r="C214" s="13"/>
+      <c r="D214" s="5">
+        <v>156184812</v>
+      </c>
+      <c r="E214" s="5">
+        <v>156650711</v>
+      </c>
+      <c r="F214" s="11"/>
+      <c r="G214" s="11"/>
+      <c r="H214" s="11"/>
+      <c r="I214" s="2"/>
+      <c r="J214" s="2"/>
+      <c r="K214" s="2"/>
+      <c r="L214" s="2"/>
+      <c r="M214" s="2"/>
+      <c r="N214" s="2"/>
+      <c r="O214" s="2"/>
+      <c r="P214" s="2"/>
+      <c r="Q214" s="2"/>
+      <c r="R214" s="2"/>
+      <c r="S214" s="2"/>
+      <c r="T214" s="2"/>
+      <c r="U214" s="2"/>
+      <c r="V214" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>